<commit_message>
lol fixed error in indentation in main
</commit_message>
<xml_diff>
--- a/tranchedata.xlsx
+++ b/tranchedata.xlsx
@@ -537,7 +537,7 @@
         <v>52</v>
       </c>
       <c r="C8">
-        <v>1831093.464514666</v>
+        <v>1892129.913331822</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -552,13 +552,13 @@
         <v>53</v>
       </c>
       <c r="C9">
-        <v>1831093.464514666</v>
+        <v>1892129.913331822</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>65221702.36000001</v>
       </c>
       <c r="E9">
-        <v>346579204.64</v>
+        <v>281357502.28</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -567,13 +567,13 @@
         <v>54</v>
       </c>
       <c r="C10">
-        <v>1831093.464514666</v>
+        <v>1387405.105687378</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>55000000</v>
       </c>
       <c r="E10">
-        <v>346579204.64</v>
+        <v>226357502.28</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -582,13 +582,13 @@
         <v>55</v>
       </c>
       <c r="C11">
-        <v>1831093.464514666</v>
+        <v>1235786.208280866</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>58111292.09213597</v>
       </c>
       <c r="E11">
-        <v>346579204.64</v>
+        <v>168246210.187864</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -597,13 +597,13 @@
         <v>56</v>
       </c>
       <c r="C12">
-        <v>1831093.464514666</v>
+        <v>888900.8104925482</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12">
-        <v>346579204.64</v>
+        <v>168246210.187864</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -612,13 +612,13 @@
         <v>57</v>
       </c>
       <c r="C13">
-        <v>1831093.464514666</v>
+        <v>918530.8375089663</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>143686931.94</v>
       </c>
       <c r="E13">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -627,13 +627,13 @@
         <v>58</v>
       </c>
       <c r="C14">
-        <v>1831093.464514666</v>
+        <v>129754.8534095481</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -642,13 +642,13 @@
         <v>59</v>
       </c>
       <c r="C15">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D15">
         <v>0</v>
       </c>
       <c r="E15">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -657,13 +657,13 @@
         <v>60</v>
       </c>
       <c r="C16">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -672,13 +672,13 @@
         <v>61</v>
       </c>
       <c r="C17">
-        <v>1831093.464514666</v>
+        <v>129754.8534095481</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -687,13 +687,13 @@
         <v>62</v>
       </c>
       <c r="C18">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -702,13 +702,13 @@
         <v>63</v>
       </c>
       <c r="C19">
-        <v>1831093.464514666</v>
+        <v>129754.8534095481</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -717,13 +717,13 @@
         <v>64</v>
       </c>
       <c r="C20">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -732,13 +732,13 @@
         <v>65</v>
       </c>
       <c r="C21">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -747,13 +747,13 @@
         <v>66</v>
       </c>
       <c r="C22">
-        <v>1831093.464514666</v>
+        <v>121104.5298489115</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -762,13 +762,13 @@
         <v>67</v>
       </c>
       <c r="C23">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -777,13 +777,13 @@
         <v>68</v>
       </c>
       <c r="C24">
-        <v>1831093.464514666</v>
+        <v>129754.8534095481</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -792,13 +792,13 @@
         <v>69</v>
       </c>
       <c r="C25">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -807,13 +807,13 @@
         <v>70</v>
       </c>
       <c r="C26">
-        <v>1831093.464514666</v>
+        <v>129754.8534095481</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -822,13 +822,13 @@
         <v>71</v>
       </c>
       <c r="C27">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
       <c r="E27">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -837,13 +837,13 @@
         <v>72</v>
       </c>
       <c r="C28">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
       <c r="E28">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -852,13 +852,13 @@
         <v>73</v>
       </c>
       <c r="C29">
-        <v>1831093.464514666</v>
+        <v>129754.8534095481</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -867,13 +867,13 @@
         <v>74</v>
       </c>
       <c r="C30">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -882,13 +882,13 @@
         <v>75</v>
       </c>
       <c r="C31">
-        <v>1831093.464514666</v>
+        <v>129754.8534095481</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="E31">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -897,13 +897,13 @@
         <v>76</v>
       </c>
       <c r="C32">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D32">
         <v>0</v>
       </c>
       <c r="E32">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -912,13 +912,13 @@
         <v>77</v>
       </c>
       <c r="C33">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D33">
         <v>0</v>
       </c>
       <c r="E33">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -927,13 +927,13 @@
         <v>78</v>
       </c>
       <c r="C34">
-        <v>1831093.464514666</v>
+        <v>121104.5298489115</v>
       </c>
       <c r="D34">
         <v>0</v>
       </c>
       <c r="E34">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -942,13 +942,13 @@
         <v>79</v>
       </c>
       <c r="C35">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="E35">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -957,13 +957,13 @@
         <v>80</v>
       </c>
       <c r="C36">
-        <v>1831093.464514666</v>
+        <v>129754.8534095481</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="E36">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -972,13 +972,13 @@
         <v>81</v>
       </c>
       <c r="C37">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
       <c r="E37">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -987,13 +987,13 @@
         <v>82</v>
       </c>
       <c r="C38">
-        <v>1831093.464514666</v>
+        <v>129754.8534095481</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
       <c r="E38">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1002,13 +1002,13 @@
         <v>83</v>
       </c>
       <c r="C39">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D39">
         <v>0</v>
       </c>
       <c r="E39">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1017,13 +1017,13 @@
         <v>84</v>
       </c>
       <c r="C40">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D40">
         <v>0</v>
       </c>
       <c r="E40">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1032,13 +1032,13 @@
         <v>85</v>
       </c>
       <c r="C41">
-        <v>1831093.464514666</v>
+        <v>129754.8534095481</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
       <c r="E41">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1047,13 +1047,13 @@
         <v>86</v>
       </c>
       <c r="C42">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
       <c r="E42">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1062,13 +1062,13 @@
         <v>87</v>
       </c>
       <c r="C43">
-        <v>1831093.464514666</v>
+        <v>129754.8534095481</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="E43">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1077,13 +1077,13 @@
         <v>88</v>
       </c>
       <c r="C44">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D44">
         <v>0</v>
       </c>
       <c r="E44">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1092,13 +1092,13 @@
         <v>89</v>
       </c>
       <c r="C45">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D45">
         <v>0</v>
       </c>
       <c r="E45">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1107,13 +1107,13 @@
         <v>90</v>
       </c>
       <c r="C46">
-        <v>1831093.464514666</v>
+        <v>121104.5298489115</v>
       </c>
       <c r="D46">
         <v>0</v>
       </c>
       <c r="E46">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1122,13 +1122,13 @@
         <v>91</v>
       </c>
       <c r="C47">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D47">
         <v>0</v>
       </c>
       <c r="E47">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1137,13 +1137,13 @@
         <v>92</v>
       </c>
       <c r="C48">
-        <v>1831093.464514666</v>
+        <v>129754.8534095481</v>
       </c>
       <c r="D48">
         <v>0</v>
       </c>
       <c r="E48">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1152,13 +1152,13 @@
         <v>93</v>
       </c>
       <c r="C49">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D49">
         <v>0</v>
       </c>
       <c r="E49">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1167,13 +1167,13 @@
         <v>94</v>
       </c>
       <c r="C50">
-        <v>1831093.464514666</v>
+        <v>129754.8534095481</v>
       </c>
       <c r="D50">
         <v>0</v>
       </c>
       <c r="E50">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1182,13 +1182,13 @@
         <v>95</v>
       </c>
       <c r="C51">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D51">
         <v>0</v>
       </c>
       <c r="E51">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1197,13 +1197,13 @@
         <v>96</v>
       </c>
       <c r="C52">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D52">
         <v>0</v>
       </c>
       <c r="E52">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1212,13 +1212,13 @@
         <v>97</v>
       </c>
       <c r="C53">
-        <v>1831093.464514666</v>
+        <v>129754.8534095481</v>
       </c>
       <c r="D53">
         <v>0</v>
       </c>
       <c r="E53">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1227,13 +1227,13 @@
         <v>98</v>
       </c>
       <c r="C54">
-        <v>1831093.464514666</v>
+        <v>134080.0151898663</v>
       </c>
       <c r="D54">
         <v>0</v>
       </c>
       <c r="E54">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1242,13 +1242,13 @@
         <v>99</v>
       </c>
       <c r="C55">
-        <v>1831093.464514666</v>
+        <v>129754.8534095481</v>
       </c>
       <c r="D55">
         <v>0</v>
       </c>
       <c r="E55">
-        <v>346579204.64</v>
+        <v>24559278.24786399</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1349,7 +1349,7 @@
         <v>52</v>
       </c>
       <c r="C62">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -1364,7 +1364,7 @@
         <v>53</v>
       </c>
       <c r="C63">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -1379,7 +1379,7 @@
         <v>54</v>
       </c>
       <c r="C64">
-        <v>786018.7499999999</v>
+        <v>733617.4999999999</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -1394,7 +1394,7 @@
         <v>55</v>
       </c>
       <c r="C65">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -1424,7 +1424,7 @@
         <v>57</v>
       </c>
       <c r="C67">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -1454,7 +1454,7 @@
         <v>59</v>
       </c>
       <c r="C69">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -1469,7 +1469,7 @@
         <v>60</v>
       </c>
       <c r="C70">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -1499,7 +1499,7 @@
         <v>62</v>
       </c>
       <c r="C72">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -1529,7 +1529,7 @@
         <v>64</v>
       </c>
       <c r="C74">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -1544,7 +1544,7 @@
         <v>65</v>
       </c>
       <c r="C75">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -1559,7 +1559,7 @@
         <v>66</v>
       </c>
       <c r="C76">
-        <v>786018.7499999999</v>
+        <v>733617.4999999999</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -1574,7 +1574,7 @@
         <v>67</v>
       </c>
       <c r="C77">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -1604,7 +1604,7 @@
         <v>69</v>
       </c>
       <c r="C79">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -1634,7 +1634,7 @@
         <v>71</v>
       </c>
       <c r="C81">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -1649,7 +1649,7 @@
         <v>72</v>
       </c>
       <c r="C82">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -1679,7 +1679,7 @@
         <v>74</v>
       </c>
       <c r="C84">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -1709,7 +1709,7 @@
         <v>76</v>
       </c>
       <c r="C86">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -1724,7 +1724,7 @@
         <v>77</v>
       </c>
       <c r="C87">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -1739,7 +1739,7 @@
         <v>78</v>
       </c>
       <c r="C88">
-        <v>786018.7499999999</v>
+        <v>733617.4999999999</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -1754,7 +1754,7 @@
         <v>79</v>
       </c>
       <c r="C89">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -1784,7 +1784,7 @@
         <v>81</v>
       </c>
       <c r="C91">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -1814,7 +1814,7 @@
         <v>83</v>
       </c>
       <c r="C93">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D93">
         <v>0</v>
@@ -1829,7 +1829,7 @@
         <v>84</v>
       </c>
       <c r="C94">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -1859,7 +1859,7 @@
         <v>86</v>
       </c>
       <c r="C96">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -1889,7 +1889,7 @@
         <v>88</v>
       </c>
       <c r="C98">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D98">
         <v>0</v>
@@ -1904,7 +1904,7 @@
         <v>89</v>
       </c>
       <c r="C99">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -1919,7 +1919,7 @@
         <v>90</v>
       </c>
       <c r="C100">
-        <v>786018.7499999999</v>
+        <v>733617.4999999999</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -1934,7 +1934,7 @@
         <v>91</v>
       </c>
       <c r="C101">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -1964,7 +1964,7 @@
         <v>93</v>
       </c>
       <c r="C103">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D103">
         <v>0</v>
@@ -1994,7 +1994,7 @@
         <v>95</v>
       </c>
       <c r="C105">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D105">
         <v>0</v>
@@ -2009,7 +2009,7 @@
         <v>96</v>
       </c>
       <c r="C106">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D106">
         <v>0</v>
@@ -2039,7 +2039,7 @@
         <v>98</v>
       </c>
       <c r="C108">
-        <v>786018.7499999999</v>
+        <v>812219.3749999999</v>
       </c>
       <c r="D108">
         <v>0</v>
@@ -2161,7 +2161,7 @@
         <v>52</v>
       </c>
       <c r="C116">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D116">
         <v>0</v>
@@ -2176,7 +2176,7 @@
         <v>53</v>
       </c>
       <c r="C117">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D117">
         <v>0</v>
@@ -2191,7 +2191,7 @@
         <v>54</v>
       </c>
       <c r="C118">
-        <v>377300</v>
+        <v>352146.6666666667</v>
       </c>
       <c r="D118">
         <v>0</v>
@@ -2206,7 +2206,7 @@
         <v>55</v>
       </c>
       <c r="C119">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D119">
         <v>0</v>
@@ -2236,7 +2236,7 @@
         <v>57</v>
       </c>
       <c r="C121">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D121">
         <v>0</v>
@@ -2266,7 +2266,7 @@
         <v>59</v>
       </c>
       <c r="C123">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D123">
         <v>0</v>
@@ -2281,7 +2281,7 @@
         <v>60</v>
       </c>
       <c r="C124">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D124">
         <v>0</v>
@@ -2311,7 +2311,7 @@
         <v>62</v>
       </c>
       <c r="C126">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D126">
         <v>0</v>
@@ -2341,7 +2341,7 @@
         <v>64</v>
       </c>
       <c r="C128">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D128">
         <v>0</v>
@@ -2356,7 +2356,7 @@
         <v>65</v>
       </c>
       <c r="C129">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D129">
         <v>0</v>
@@ -2371,7 +2371,7 @@
         <v>66</v>
       </c>
       <c r="C130">
-        <v>377300</v>
+        <v>352146.6666666667</v>
       </c>
       <c r="D130">
         <v>0</v>
@@ -2386,7 +2386,7 @@
         <v>67</v>
       </c>
       <c r="C131">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D131">
         <v>0</v>
@@ -2416,7 +2416,7 @@
         <v>69</v>
       </c>
       <c r="C133">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D133">
         <v>0</v>
@@ -2446,7 +2446,7 @@
         <v>71</v>
       </c>
       <c r="C135">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D135">
         <v>0</v>
@@ -2461,7 +2461,7 @@
         <v>72</v>
       </c>
       <c r="C136">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D136">
         <v>0</v>
@@ -2491,7 +2491,7 @@
         <v>74</v>
       </c>
       <c r="C138">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D138">
         <v>0</v>
@@ -2521,7 +2521,7 @@
         <v>76</v>
       </c>
       <c r="C140">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D140">
         <v>0</v>
@@ -2536,7 +2536,7 @@
         <v>77</v>
       </c>
       <c r="C141">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D141">
         <v>0</v>
@@ -2551,7 +2551,7 @@
         <v>78</v>
       </c>
       <c r="C142">
-        <v>377300</v>
+        <v>352146.6666666667</v>
       </c>
       <c r="D142">
         <v>0</v>
@@ -2566,7 +2566,7 @@
         <v>79</v>
       </c>
       <c r="C143">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D143">
         <v>0</v>
@@ -2596,7 +2596,7 @@
         <v>81</v>
       </c>
       <c r="C145">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D145">
         <v>0</v>
@@ -2626,7 +2626,7 @@
         <v>83</v>
       </c>
       <c r="C147">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D147">
         <v>0</v>
@@ -2641,7 +2641,7 @@
         <v>84</v>
       </c>
       <c r="C148">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D148">
         <v>0</v>
@@ -2671,7 +2671,7 @@
         <v>86</v>
       </c>
       <c r="C150">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D150">
         <v>0</v>
@@ -2701,7 +2701,7 @@
         <v>88</v>
       </c>
       <c r="C152">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D152">
         <v>0</v>
@@ -2716,7 +2716,7 @@
         <v>89</v>
       </c>
       <c r="C153">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D153">
         <v>0</v>
@@ -2731,7 +2731,7 @@
         <v>90</v>
       </c>
       <c r="C154">
-        <v>377300</v>
+        <v>352146.6666666667</v>
       </c>
       <c r="D154">
         <v>0</v>
@@ -2746,7 +2746,7 @@
         <v>91</v>
       </c>
       <c r="C155">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D155">
         <v>0</v>
@@ -2776,7 +2776,7 @@
         <v>93</v>
       </c>
       <c r="C157">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D157">
         <v>0</v>
@@ -2806,7 +2806,7 @@
         <v>95</v>
       </c>
       <c r="C159">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D159">
         <v>0</v>
@@ -2821,7 +2821,7 @@
         <v>96</v>
       </c>
       <c r="C160">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D160">
         <v>0</v>
@@ -2851,7 +2851,7 @@
         <v>98</v>
       </c>
       <c r="C162">
-        <v>377300</v>
+        <v>389876.6666666667</v>
       </c>
       <c r="D162">
         <v>0</v>
@@ -2973,7 +2973,7 @@
         <v>52</v>
       </c>
       <c r="C170">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D170">
         <v>0</v>
@@ -2988,7 +2988,7 @@
         <v>53</v>
       </c>
       <c r="C171">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D171">
         <v>0</v>
@@ -3003,7 +3003,7 @@
         <v>54</v>
       </c>
       <c r="C172">
-        <v>479164.5833333333</v>
+        <v>447220.2777777778</v>
       </c>
       <c r="D172">
         <v>0</v>
@@ -3018,7 +3018,7 @@
         <v>55</v>
       </c>
       <c r="C173">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D173">
         <v>0</v>
@@ -3048,7 +3048,7 @@
         <v>57</v>
       </c>
       <c r="C175">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D175">
         <v>0</v>
@@ -3078,7 +3078,7 @@
         <v>59</v>
       </c>
       <c r="C177">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D177">
         <v>0</v>
@@ -3093,7 +3093,7 @@
         <v>60</v>
       </c>
       <c r="C178">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D178">
         <v>0</v>
@@ -3123,7 +3123,7 @@
         <v>62</v>
       </c>
       <c r="C180">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D180">
         <v>0</v>
@@ -3153,7 +3153,7 @@
         <v>64</v>
       </c>
       <c r="C182">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D182">
         <v>0</v>
@@ -3168,7 +3168,7 @@
         <v>65</v>
       </c>
       <c r="C183">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D183">
         <v>0</v>
@@ -3183,7 +3183,7 @@
         <v>66</v>
       </c>
       <c r="C184">
-        <v>479164.5833333333</v>
+        <v>447220.2777777778</v>
       </c>
       <c r="D184">
         <v>0</v>
@@ -3198,7 +3198,7 @@
         <v>67</v>
       </c>
       <c r="C185">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D185">
         <v>0</v>
@@ -3228,7 +3228,7 @@
         <v>69</v>
       </c>
       <c r="C187">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D187">
         <v>0</v>
@@ -3258,7 +3258,7 @@
         <v>71</v>
       </c>
       <c r="C189">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D189">
         <v>0</v>
@@ -3273,7 +3273,7 @@
         <v>72</v>
       </c>
       <c r="C190">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D190">
         <v>0</v>
@@ -3303,7 +3303,7 @@
         <v>74</v>
       </c>
       <c r="C192">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D192">
         <v>0</v>
@@ -3333,7 +3333,7 @@
         <v>76</v>
       </c>
       <c r="C194">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D194">
         <v>0</v>
@@ -3348,7 +3348,7 @@
         <v>77</v>
       </c>
       <c r="C195">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D195">
         <v>0</v>
@@ -3363,7 +3363,7 @@
         <v>78</v>
       </c>
       <c r="C196">
-        <v>479164.5833333333</v>
+        <v>447220.2777777778</v>
       </c>
       <c r="D196">
         <v>0</v>
@@ -3378,7 +3378,7 @@
         <v>79</v>
       </c>
       <c r="C197">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D197">
         <v>0</v>
@@ -3408,7 +3408,7 @@
         <v>81</v>
       </c>
       <c r="C199">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D199">
         <v>0</v>
@@ -3438,7 +3438,7 @@
         <v>83</v>
       </c>
       <c r="C201">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D201">
         <v>0</v>
@@ -3453,7 +3453,7 @@
         <v>84</v>
       </c>
       <c r="C202">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D202">
         <v>0</v>
@@ -3483,7 +3483,7 @@
         <v>86</v>
       </c>
       <c r="C204">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D204">
         <v>0</v>
@@ -3513,7 +3513,7 @@
         <v>88</v>
       </c>
       <c r="C206">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D206">
         <v>0</v>
@@ -3528,7 +3528,7 @@
         <v>89</v>
       </c>
       <c r="C207">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D207">
         <v>0</v>
@@ -3543,7 +3543,7 @@
         <v>90</v>
       </c>
       <c r="C208">
-        <v>479164.5833333333</v>
+        <v>447220.2777777778</v>
       </c>
       <c r="D208">
         <v>0</v>
@@ -3558,7 +3558,7 @@
         <v>91</v>
       </c>
       <c r="C209">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D209">
         <v>0</v>
@@ -3588,7 +3588,7 @@
         <v>93</v>
       </c>
       <c r="C211">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D211">
         <v>0</v>
@@ -3618,7 +3618,7 @@
         <v>95</v>
       </c>
       <c r="C213">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D213">
         <v>0</v>
@@ -3633,7 +3633,7 @@
         <v>96</v>
       </c>
       <c r="C214">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D214">
         <v>0</v>
@@ -3663,7 +3663,7 @@
         <v>98</v>
       </c>
       <c r="C216">
-        <v>479164.5833333333</v>
+        <v>495136.7361111111</v>
       </c>
       <c r="D216">
         <v>0</v>
@@ -3785,7 +3785,7 @@
         <v>52</v>
       </c>
       <c r="C224">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D224">
         <v>0</v>
@@ -3800,7 +3800,7 @@
         <v>53</v>
       </c>
       <c r="C225">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D225">
         <v>0</v>
@@ -3815,7 +3815,7 @@
         <v>54</v>
       </c>
       <c r="C226">
-        <v>374951.0416666667</v>
+        <v>349954.3055555556</v>
       </c>
       <c r="D226">
         <v>0</v>
@@ -3830,7 +3830,7 @@
         <v>55</v>
       </c>
       <c r="C227">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D227">
         <v>0</v>
@@ -3860,7 +3860,7 @@
         <v>57</v>
       </c>
       <c r="C229">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D229">
         <v>0</v>
@@ -3890,7 +3890,7 @@
         <v>59</v>
       </c>
       <c r="C231">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D231">
         <v>0</v>
@@ -3905,7 +3905,7 @@
         <v>60</v>
       </c>
       <c r="C232">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D232">
         <v>0</v>
@@ -3935,7 +3935,7 @@
         <v>62</v>
       </c>
       <c r="C234">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D234">
         <v>0</v>
@@ -3965,7 +3965,7 @@
         <v>64</v>
       </c>
       <c r="C236">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D236">
         <v>0</v>
@@ -3980,7 +3980,7 @@
         <v>65</v>
       </c>
       <c r="C237">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D237">
         <v>0</v>
@@ -3995,7 +3995,7 @@
         <v>66</v>
       </c>
       <c r="C238">
-        <v>374951.0416666667</v>
+        <v>349954.3055555556</v>
       </c>
       <c r="D238">
         <v>0</v>
@@ -4010,7 +4010,7 @@
         <v>67</v>
       </c>
       <c r="C239">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D239">
         <v>0</v>
@@ -4040,7 +4040,7 @@
         <v>69</v>
       </c>
       <c r="C241">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D241">
         <v>0</v>
@@ -4070,7 +4070,7 @@
         <v>71</v>
       </c>
       <c r="C243">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D243">
         <v>0</v>
@@ -4085,7 +4085,7 @@
         <v>72</v>
       </c>
       <c r="C244">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D244">
         <v>0</v>
@@ -4115,7 +4115,7 @@
         <v>74</v>
       </c>
       <c r="C246">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D246">
         <v>0</v>
@@ -4145,7 +4145,7 @@
         <v>76</v>
       </c>
       <c r="C248">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D248">
         <v>0</v>
@@ -4160,7 +4160,7 @@
         <v>77</v>
       </c>
       <c r="C249">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D249">
         <v>0</v>
@@ -4175,7 +4175,7 @@
         <v>78</v>
       </c>
       <c r="C250">
-        <v>374951.0416666667</v>
+        <v>349954.3055555556</v>
       </c>
       <c r="D250">
         <v>0</v>
@@ -4190,7 +4190,7 @@
         <v>79</v>
       </c>
       <c r="C251">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D251">
         <v>0</v>
@@ -4220,7 +4220,7 @@
         <v>81</v>
       </c>
       <c r="C253">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D253">
         <v>0</v>
@@ -4250,7 +4250,7 @@
         <v>83</v>
       </c>
       <c r="C255">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D255">
         <v>0</v>
@@ -4265,7 +4265,7 @@
         <v>84</v>
       </c>
       <c r="C256">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D256">
         <v>0</v>
@@ -4295,7 +4295,7 @@
         <v>86</v>
       </c>
       <c r="C258">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D258">
         <v>0</v>
@@ -4325,7 +4325,7 @@
         <v>88</v>
       </c>
       <c r="C260">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D260">
         <v>0</v>
@@ -4340,7 +4340,7 @@
         <v>89</v>
       </c>
       <c r="C261">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D261">
         <v>0</v>
@@ -4355,7 +4355,7 @@
         <v>90</v>
       </c>
       <c r="C262">
-        <v>374951.0416666667</v>
+        <v>349954.3055555556</v>
       </c>
       <c r="D262">
         <v>0</v>
@@ -4370,7 +4370,7 @@
         <v>91</v>
       </c>
       <c r="C263">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D263">
         <v>0</v>
@@ -4400,7 +4400,7 @@
         <v>93</v>
       </c>
       <c r="C265">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D265">
         <v>0</v>
@@ -4430,7 +4430,7 @@
         <v>95</v>
       </c>
       <c r="C267">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D267">
         <v>0</v>
@@ -4445,7 +4445,7 @@
         <v>96</v>
       </c>
       <c r="C268">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D268">
         <v>0</v>
@@ -4475,7 +4475,7 @@
         <v>98</v>
       </c>
       <c r="C270">
-        <v>374951.0416666667</v>
+        <v>387449.4097222222</v>
       </c>
       <c r="D270">
         <v>0</v>
@@ -4597,7 +4597,7 @@
         <v>52</v>
       </c>
       <c r="C278">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D278">
         <v>0</v>
@@ -4612,7 +4612,7 @@
         <v>53</v>
       </c>
       <c r="C279">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D279">
         <v>0</v>
@@ -4627,7 +4627,7 @@
         <v>54</v>
       </c>
       <c r="C280">
-        <v>82087.5</v>
+        <v>76615</v>
       </c>
       <c r="D280">
         <v>0</v>
@@ -4642,7 +4642,7 @@
         <v>55</v>
       </c>
       <c r="C281">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D281">
         <v>0</v>
@@ -4672,7 +4672,7 @@
         <v>57</v>
       </c>
       <c r="C283">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D283">
         <v>0</v>
@@ -4702,7 +4702,7 @@
         <v>59</v>
       </c>
       <c r="C285">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D285">
         <v>0</v>
@@ -4717,7 +4717,7 @@
         <v>60</v>
       </c>
       <c r="C286">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D286">
         <v>0</v>
@@ -4747,7 +4747,7 @@
         <v>62</v>
       </c>
       <c r="C288">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D288">
         <v>0</v>
@@ -4777,7 +4777,7 @@
         <v>64</v>
       </c>
       <c r="C290">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D290">
         <v>0</v>
@@ -4792,7 +4792,7 @@
         <v>65</v>
       </c>
       <c r="C291">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D291">
         <v>0</v>
@@ -4807,7 +4807,7 @@
         <v>66</v>
       </c>
       <c r="C292">
-        <v>82087.5</v>
+        <v>76615</v>
       </c>
       <c r="D292">
         <v>0</v>
@@ -4822,7 +4822,7 @@
         <v>67</v>
       </c>
       <c r="C293">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D293">
         <v>0</v>
@@ -4852,7 +4852,7 @@
         <v>69</v>
       </c>
       <c r="C295">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D295">
         <v>0</v>
@@ -4882,7 +4882,7 @@
         <v>71</v>
       </c>
       <c r="C297">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D297">
         <v>0</v>
@@ -4897,7 +4897,7 @@
         <v>72</v>
       </c>
       <c r="C298">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D298">
         <v>0</v>
@@ -4927,7 +4927,7 @@
         <v>74</v>
       </c>
       <c r="C300">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D300">
         <v>0</v>
@@ -4957,7 +4957,7 @@
         <v>76</v>
       </c>
       <c r="C302">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D302">
         <v>0</v>
@@ -4972,7 +4972,7 @@
         <v>77</v>
       </c>
       <c r="C303">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D303">
         <v>0</v>
@@ -4987,7 +4987,7 @@
         <v>78</v>
       </c>
       <c r="C304">
-        <v>82087.5</v>
+        <v>76615</v>
       </c>
       <c r="D304">
         <v>0</v>
@@ -5002,7 +5002,7 @@
         <v>79</v>
       </c>
       <c r="C305">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D305">
         <v>0</v>
@@ -5032,7 +5032,7 @@
         <v>81</v>
       </c>
       <c r="C307">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D307">
         <v>0</v>
@@ -5062,7 +5062,7 @@
         <v>83</v>
       </c>
       <c r="C309">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D309">
         <v>0</v>
@@ -5077,7 +5077,7 @@
         <v>84</v>
       </c>
       <c r="C310">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D310">
         <v>0</v>
@@ -5107,7 +5107,7 @@
         <v>86</v>
       </c>
       <c r="C312">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D312">
         <v>0</v>
@@ -5137,7 +5137,7 @@
         <v>88</v>
       </c>
       <c r="C314">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D314">
         <v>0</v>
@@ -5152,7 +5152,7 @@
         <v>89</v>
       </c>
       <c r="C315">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D315">
         <v>0</v>
@@ -5167,7 +5167,7 @@
         <v>90</v>
       </c>
       <c r="C316">
-        <v>82087.5</v>
+        <v>76615</v>
       </c>
       <c r="D316">
         <v>0</v>
@@ -5182,7 +5182,7 @@
         <v>91</v>
       </c>
       <c r="C317">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D317">
         <v>0</v>
@@ -5212,7 +5212,7 @@
         <v>93</v>
       </c>
       <c r="C319">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D319">
         <v>0</v>
@@ -5242,7 +5242,7 @@
         <v>95</v>
       </c>
       <c r="C321">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D321">
         <v>0</v>
@@ -5257,7 +5257,7 @@
         <v>96</v>
       </c>
       <c r="C322">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D322">
         <v>0</v>
@@ -5287,7 +5287,7 @@
         <v>98</v>
       </c>
       <c r="C324">
-        <v>82087.5</v>
+        <v>84823.75</v>
       </c>
       <c r="D324">
         <v>0</v>
@@ -5590,6 +5590,9 @@
       <c r="B342" s="1">
         <v>51</v>
       </c>
+      <c r="C342">
+        <v>0</v>
+      </c>
       <c r="D342">
         <v>0</v>
       </c>
@@ -5604,6 +5607,9 @@
       <c r="B343" s="1">
         <v>51</v>
       </c>
+      <c r="C343">
+        <v>0</v>
+      </c>
       <c r="D343">
         <v>0</v>
       </c>
@@ -5618,6 +5624,9 @@
       <c r="B344" s="1">
         <v>51</v>
       </c>
+      <c r="C344">
+        <v>0</v>
+      </c>
       <c r="D344">
         <v>0</v>
       </c>
@@ -5632,6 +5641,9 @@
       <c r="B345" s="1">
         <v>51</v>
       </c>
+      <c r="C345">
+        <v>0</v>
+      </c>
       <c r="D345">
         <v>0</v>
       </c>
@@ -5646,6 +5658,9 @@
       <c r="B346" s="1">
         <v>52</v>
       </c>
+      <c r="C346">
+        <v>0</v>
+      </c>
       <c r="D346">
         <v>0</v>
       </c>
@@ -5660,6 +5675,9 @@
       <c r="B347" s="1">
         <v>52</v>
       </c>
+      <c r="C347">
+        <v>0</v>
+      </c>
       <c r="D347">
         <v>0</v>
       </c>
@@ -5674,6 +5692,9 @@
       <c r="B348" s="1">
         <v>52</v>
       </c>
+      <c r="C348">
+        <v>0</v>
+      </c>
       <c r="D348">
         <v>0</v>
       </c>
@@ -5688,6 +5709,9 @@
       <c r="B349" s="1">
         <v>52</v>
       </c>
+      <c r="C349">
+        <v>0</v>
+      </c>
       <c r="D349">
         <v>0</v>
       </c>
@@ -5702,6 +5726,9 @@
       <c r="B350" s="1">
         <v>53</v>
       </c>
+      <c r="C350">
+        <v>0</v>
+      </c>
       <c r="D350">
         <v>0</v>
       </c>
@@ -5716,6 +5743,9 @@
       <c r="B351" s="1">
         <v>53</v>
       </c>
+      <c r="C351">
+        <v>0</v>
+      </c>
       <c r="D351">
         <v>0</v>
       </c>
@@ -5730,6 +5760,9 @@
       <c r="B352" s="1">
         <v>53</v>
       </c>
+      <c r="C352">
+        <v>0</v>
+      </c>
       <c r="D352">
         <v>0</v>
       </c>
@@ -5744,6 +5777,9 @@
       <c r="B353" s="1">
         <v>53</v>
       </c>
+      <c r="C353">
+        <v>0</v>
+      </c>
       <c r="D353">
         <v>0</v>
       </c>
@@ -5758,6 +5794,9 @@
       <c r="B354" s="1">
         <v>54</v>
       </c>
+      <c r="C354">
+        <v>0</v>
+      </c>
       <c r="D354">
         <v>0</v>
       </c>
@@ -5772,6 +5811,9 @@
       <c r="B355" s="1">
         <v>54</v>
       </c>
+      <c r="C355">
+        <v>0</v>
+      </c>
       <c r="D355">
         <v>0</v>
       </c>
@@ -5786,6 +5828,9 @@
       <c r="B356" s="1">
         <v>54</v>
       </c>
+      <c r="C356">
+        <v>0</v>
+      </c>
       <c r="D356">
         <v>0</v>
       </c>
@@ -5800,6 +5845,9 @@
       <c r="B357" s="1">
         <v>54</v>
       </c>
+      <c r="C357">
+        <v>0</v>
+      </c>
       <c r="D357">
         <v>0</v>
       </c>
@@ -5814,6 +5862,9 @@
       <c r="B358" s="1">
         <v>55</v>
       </c>
+      <c r="C358">
+        <v>0</v>
+      </c>
       <c r="D358">
         <v>0</v>
       </c>
@@ -5828,6 +5879,9 @@
       <c r="B359" s="1">
         <v>55</v>
       </c>
+      <c r="C359">
+        <v>0</v>
+      </c>
       <c r="D359">
         <v>0</v>
       </c>
@@ -5842,6 +5896,9 @@
       <c r="B360" s="1">
         <v>55</v>
       </c>
+      <c r="C360">
+        <v>0</v>
+      </c>
       <c r="D360">
         <v>0</v>
       </c>
@@ -5856,6 +5913,9 @@
       <c r="B361" s="1">
         <v>55</v>
       </c>
+      <c r="C361">
+        <v>0</v>
+      </c>
       <c r="D361">
         <v>0</v>
       </c>
@@ -5870,6 +5930,9 @@
       <c r="B362" s="1">
         <v>56</v>
       </c>
+      <c r="C362">
+        <v>0</v>
+      </c>
       <c r="D362">
         <v>0</v>
       </c>
@@ -5884,6 +5947,9 @@
       <c r="B363" s="1">
         <v>56</v>
       </c>
+      <c r="C363">
+        <v>0</v>
+      </c>
       <c r="D363">
         <v>0</v>
       </c>
@@ -5898,6 +5964,9 @@
       <c r="B364" s="1">
         <v>56</v>
       </c>
+      <c r="C364">
+        <v>0</v>
+      </c>
       <c r="D364">
         <v>0</v>
       </c>
@@ -5912,6 +5981,9 @@
       <c r="B365" s="1">
         <v>56</v>
       </c>
+      <c r="C365">
+        <v>0</v>
+      </c>
       <c r="D365">
         <v>0</v>
       </c>
@@ -5926,6 +5998,9 @@
       <c r="B366" s="1">
         <v>57</v>
       </c>
+      <c r="C366">
+        <v>0</v>
+      </c>
       <c r="D366">
         <v>0</v>
       </c>
@@ -5940,6 +6015,9 @@
       <c r="B367" s="1">
         <v>57</v>
       </c>
+      <c r="C367">
+        <v>0</v>
+      </c>
       <c r="D367">
         <v>0</v>
       </c>
@@ -5954,6 +6032,9 @@
       <c r="B368" s="1">
         <v>57</v>
       </c>
+      <c r="C368">
+        <v>0</v>
+      </c>
       <c r="D368">
         <v>0</v>
       </c>
@@ -5968,6 +6049,9 @@
       <c r="B369" s="1">
         <v>57</v>
       </c>
+      <c r="C369">
+        <v>0</v>
+      </c>
       <c r="D369">
         <v>0</v>
       </c>
@@ -5982,6 +6066,9 @@
       <c r="B370" s="1">
         <v>58</v>
       </c>
+      <c r="C370">
+        <v>0</v>
+      </c>
       <c r="D370">
         <v>0</v>
       </c>
@@ -5996,6 +6083,9 @@
       <c r="B371" s="1">
         <v>58</v>
       </c>
+      <c r="C371">
+        <v>0</v>
+      </c>
       <c r="D371">
         <v>0</v>
       </c>
@@ -6010,6 +6100,9 @@
       <c r="B372" s="1">
         <v>58</v>
       </c>
+      <c r="C372">
+        <v>0</v>
+      </c>
       <c r="D372">
         <v>0</v>
       </c>
@@ -6024,6 +6117,9 @@
       <c r="B373" s="1">
         <v>58</v>
       </c>
+      <c r="C373">
+        <v>0</v>
+      </c>
       <c r="D373">
         <v>0</v>
       </c>
@@ -6038,6 +6134,9 @@
       <c r="B374" s="1">
         <v>59</v>
       </c>
+      <c r="C374">
+        <v>0</v>
+      </c>
       <c r="D374">
         <v>0</v>
       </c>
@@ -6052,6 +6151,9 @@
       <c r="B375" s="1">
         <v>59</v>
       </c>
+      <c r="C375">
+        <v>0</v>
+      </c>
       <c r="D375">
         <v>0</v>
       </c>
@@ -6066,6 +6168,9 @@
       <c r="B376" s="1">
         <v>59</v>
       </c>
+      <c r="C376">
+        <v>0</v>
+      </c>
       <c r="D376">
         <v>0</v>
       </c>
@@ -6080,6 +6185,9 @@
       <c r="B377" s="1">
         <v>59</v>
       </c>
+      <c r="C377">
+        <v>0</v>
+      </c>
       <c r="D377">
         <v>0</v>
       </c>
@@ -6094,6 +6202,9 @@
       <c r="B378" s="1">
         <v>60</v>
       </c>
+      <c r="C378">
+        <v>0</v>
+      </c>
       <c r="D378">
         <v>0</v>
       </c>
@@ -6108,6 +6219,9 @@
       <c r="B379" s="1">
         <v>60</v>
       </c>
+      <c r="C379">
+        <v>0</v>
+      </c>
       <c r="D379">
         <v>0</v>
       </c>
@@ -6122,6 +6236,9 @@
       <c r="B380" s="1">
         <v>60</v>
       </c>
+      <c r="C380">
+        <v>0</v>
+      </c>
       <c r="D380">
         <v>0</v>
       </c>
@@ -6136,6 +6253,9 @@
       <c r="B381" s="1">
         <v>60</v>
       </c>
+      <c r="C381">
+        <v>0</v>
+      </c>
       <c r="D381">
         <v>0</v>
       </c>
@@ -6150,6 +6270,9 @@
       <c r="B382" s="1">
         <v>61</v>
       </c>
+      <c r="C382">
+        <v>0</v>
+      </c>
       <c r="D382">
         <v>0</v>
       </c>
@@ -6164,6 +6287,9 @@
       <c r="B383" s="1">
         <v>61</v>
       </c>
+      <c r="C383">
+        <v>0</v>
+      </c>
       <c r="D383">
         <v>0</v>
       </c>
@@ -6178,6 +6304,9 @@
       <c r="B384" s="1">
         <v>61</v>
       </c>
+      <c r="C384">
+        <v>0</v>
+      </c>
       <c r="D384">
         <v>0</v>
       </c>
@@ -6192,6 +6321,9 @@
       <c r="B385" s="1">
         <v>61</v>
       </c>
+      <c r="C385">
+        <v>0</v>
+      </c>
       <c r="D385">
         <v>0</v>
       </c>
@@ -6206,6 +6338,9 @@
       <c r="B386" s="1">
         <v>62</v>
       </c>
+      <c r="C386">
+        <v>0</v>
+      </c>
       <c r="D386">
         <v>0</v>
       </c>
@@ -6220,6 +6355,9 @@
       <c r="B387" s="1">
         <v>62</v>
       </c>
+      <c r="C387">
+        <v>0</v>
+      </c>
       <c r="D387">
         <v>0</v>
       </c>
@@ -6234,6 +6372,9 @@
       <c r="B388" s="1">
         <v>62</v>
       </c>
+      <c r="C388">
+        <v>0</v>
+      </c>
       <c r="D388">
         <v>0</v>
       </c>
@@ -6248,6 +6389,9 @@
       <c r="B389" s="1">
         <v>62</v>
       </c>
+      <c r="C389">
+        <v>0</v>
+      </c>
       <c r="D389">
         <v>0</v>
       </c>
@@ -6262,6 +6406,9 @@
       <c r="B390" s="1">
         <v>63</v>
       </c>
+      <c r="C390">
+        <v>0</v>
+      </c>
       <c r="D390">
         <v>0</v>
       </c>
@@ -6276,6 +6423,9 @@
       <c r="B391" s="1">
         <v>63</v>
       </c>
+      <c r="C391">
+        <v>0</v>
+      </c>
       <c r="D391">
         <v>0</v>
       </c>
@@ -6290,6 +6440,9 @@
       <c r="B392" s="1">
         <v>63</v>
       </c>
+      <c r="C392">
+        <v>0</v>
+      </c>
       <c r="D392">
         <v>0</v>
       </c>
@@ -6304,6 +6457,9 @@
       <c r="B393" s="1">
         <v>63</v>
       </c>
+      <c r="C393">
+        <v>0</v>
+      </c>
       <c r="D393">
         <v>0</v>
       </c>
@@ -6318,6 +6474,9 @@
       <c r="B394" s="1">
         <v>64</v>
       </c>
+      <c r="C394">
+        <v>0</v>
+      </c>
       <c r="D394">
         <v>0</v>
       </c>
@@ -6332,6 +6491,9 @@
       <c r="B395" s="1">
         <v>64</v>
       </c>
+      <c r="C395">
+        <v>0</v>
+      </c>
       <c r="D395">
         <v>0</v>
       </c>
@@ -6346,6 +6508,9 @@
       <c r="B396" s="1">
         <v>64</v>
       </c>
+      <c r="C396">
+        <v>0</v>
+      </c>
       <c r="D396">
         <v>0</v>
       </c>
@@ -6360,6 +6525,9 @@
       <c r="B397" s="1">
         <v>64</v>
       </c>
+      <c r="C397">
+        <v>0</v>
+      </c>
       <c r="D397">
         <v>0</v>
       </c>
@@ -6374,6 +6542,9 @@
       <c r="B398" s="1">
         <v>65</v>
       </c>
+      <c r="C398">
+        <v>0</v>
+      </c>
       <c r="D398">
         <v>0</v>
       </c>
@@ -6388,6 +6559,9 @@
       <c r="B399" s="1">
         <v>65</v>
       </c>
+      <c r="C399">
+        <v>0</v>
+      </c>
       <c r="D399">
         <v>0</v>
       </c>
@@ -6402,6 +6576,9 @@
       <c r="B400" s="1">
         <v>65</v>
       </c>
+      <c r="C400">
+        <v>0</v>
+      </c>
       <c r="D400">
         <v>0</v>
       </c>
@@ -6416,6 +6593,9 @@
       <c r="B401" s="1">
         <v>65</v>
       </c>
+      <c r="C401">
+        <v>0</v>
+      </c>
       <c r="D401">
         <v>0</v>
       </c>
@@ -6430,6 +6610,9 @@
       <c r="B402" s="1">
         <v>66</v>
       </c>
+      <c r="C402">
+        <v>0</v>
+      </c>
       <c r="D402">
         <v>0</v>
       </c>
@@ -6444,6 +6627,9 @@
       <c r="B403" s="1">
         <v>66</v>
       </c>
+      <c r="C403">
+        <v>0</v>
+      </c>
       <c r="D403">
         <v>0</v>
       </c>
@@ -6458,6 +6644,9 @@
       <c r="B404" s="1">
         <v>66</v>
       </c>
+      <c r="C404">
+        <v>0</v>
+      </c>
       <c r="D404">
         <v>0</v>
       </c>
@@ -6472,6 +6661,9 @@
       <c r="B405" s="1">
         <v>66</v>
       </c>
+      <c r="C405">
+        <v>0</v>
+      </c>
       <c r="D405">
         <v>0</v>
       </c>
@@ -6486,6 +6678,9 @@
       <c r="B406" s="1">
         <v>67</v>
       </c>
+      <c r="C406">
+        <v>0</v>
+      </c>
       <c r="D406">
         <v>0</v>
       </c>
@@ -6500,6 +6695,9 @@
       <c r="B407" s="1">
         <v>67</v>
       </c>
+      <c r="C407">
+        <v>0</v>
+      </c>
       <c r="D407">
         <v>0</v>
       </c>
@@ -6514,6 +6712,9 @@
       <c r="B408" s="1">
         <v>67</v>
       </c>
+      <c r="C408">
+        <v>0</v>
+      </c>
       <c r="D408">
         <v>0</v>
       </c>
@@ -6528,6 +6729,9 @@
       <c r="B409" s="1">
         <v>67</v>
       </c>
+      <c r="C409">
+        <v>0</v>
+      </c>
       <c r="D409">
         <v>0</v>
       </c>
@@ -6542,6 +6746,9 @@
       <c r="B410" s="1">
         <v>68</v>
       </c>
+      <c r="C410">
+        <v>0</v>
+      </c>
       <c r="D410">
         <v>0</v>
       </c>
@@ -6556,6 +6763,9 @@
       <c r="B411" s="1">
         <v>68</v>
       </c>
+      <c r="C411">
+        <v>0</v>
+      </c>
       <c r="D411">
         <v>0</v>
       </c>
@@ -6570,6 +6780,9 @@
       <c r="B412" s="1">
         <v>68</v>
       </c>
+      <c r="C412">
+        <v>0</v>
+      </c>
       <c r="D412">
         <v>0</v>
       </c>
@@ -6584,6 +6797,9 @@
       <c r="B413" s="1">
         <v>68</v>
       </c>
+      <c r="C413">
+        <v>0</v>
+      </c>
       <c r="D413">
         <v>0</v>
       </c>
@@ -6598,6 +6814,9 @@
       <c r="B414" s="1">
         <v>69</v>
       </c>
+      <c r="C414">
+        <v>0</v>
+      </c>
       <c r="D414">
         <v>0</v>
       </c>
@@ -6612,6 +6831,9 @@
       <c r="B415" s="1">
         <v>69</v>
       </c>
+      <c r="C415">
+        <v>0</v>
+      </c>
       <c r="D415">
         <v>0</v>
       </c>
@@ -6626,6 +6848,9 @@
       <c r="B416" s="1">
         <v>69</v>
       </c>
+      <c r="C416">
+        <v>0</v>
+      </c>
       <c r="D416">
         <v>0</v>
       </c>
@@ -6640,6 +6865,9 @@
       <c r="B417" s="1">
         <v>69</v>
       </c>
+      <c r="C417">
+        <v>0</v>
+      </c>
       <c r="D417">
         <v>0</v>
       </c>
@@ -6654,6 +6882,9 @@
       <c r="B418" s="1">
         <v>70</v>
       </c>
+      <c r="C418">
+        <v>0</v>
+      </c>
       <c r="D418">
         <v>0</v>
       </c>
@@ -6668,6 +6899,9 @@
       <c r="B419" s="1">
         <v>70</v>
       </c>
+      <c r="C419">
+        <v>0</v>
+      </c>
       <c r="D419">
         <v>0</v>
       </c>
@@ -6682,6 +6916,9 @@
       <c r="B420" s="1">
         <v>70</v>
       </c>
+      <c r="C420">
+        <v>0</v>
+      </c>
       <c r="D420">
         <v>0</v>
       </c>
@@ -6696,6 +6933,9 @@
       <c r="B421" s="1">
         <v>70</v>
       </c>
+      <c r="C421">
+        <v>0</v>
+      </c>
       <c r="D421">
         <v>0</v>
       </c>
@@ -6710,6 +6950,9 @@
       <c r="B422" s="1">
         <v>71</v>
       </c>
+      <c r="C422">
+        <v>0</v>
+      </c>
       <c r="D422">
         <v>0</v>
       </c>
@@ -6724,6 +6967,9 @@
       <c r="B423" s="1">
         <v>71</v>
       </c>
+      <c r="C423">
+        <v>0</v>
+      </c>
       <c r="D423">
         <v>0</v>
       </c>
@@ -6738,6 +6984,9 @@
       <c r="B424" s="1">
         <v>71</v>
       </c>
+      <c r="C424">
+        <v>0</v>
+      </c>
       <c r="D424">
         <v>0</v>
       </c>
@@ -6752,6 +7001,9 @@
       <c r="B425" s="1">
         <v>71</v>
       </c>
+      <c r="C425">
+        <v>0</v>
+      </c>
       <c r="D425">
         <v>0</v>
       </c>
@@ -6766,6 +7018,9 @@
       <c r="B426" s="1">
         <v>72</v>
       </c>
+      <c r="C426">
+        <v>0</v>
+      </c>
       <c r="D426">
         <v>0</v>
       </c>
@@ -6780,6 +7035,9 @@
       <c r="B427" s="1">
         <v>72</v>
       </c>
+      <c r="C427">
+        <v>0</v>
+      </c>
       <c r="D427">
         <v>0</v>
       </c>
@@ -6794,6 +7052,9 @@
       <c r="B428" s="1">
         <v>72</v>
       </c>
+      <c r="C428">
+        <v>0</v>
+      </c>
       <c r="D428">
         <v>0</v>
       </c>
@@ -6808,6 +7069,9 @@
       <c r="B429" s="1">
         <v>72</v>
       </c>
+      <c r="C429">
+        <v>0</v>
+      </c>
       <c r="D429">
         <v>0</v>
       </c>
@@ -6822,6 +7086,9 @@
       <c r="B430" s="1">
         <v>73</v>
       </c>
+      <c r="C430">
+        <v>0</v>
+      </c>
       <c r="D430">
         <v>0</v>
       </c>
@@ -6836,6 +7103,9 @@
       <c r="B431" s="1">
         <v>73</v>
       </c>
+      <c r="C431">
+        <v>0</v>
+      </c>
       <c r="D431">
         <v>0</v>
       </c>
@@ -6850,6 +7120,9 @@
       <c r="B432" s="1">
         <v>73</v>
       </c>
+      <c r="C432">
+        <v>0</v>
+      </c>
       <c r="D432">
         <v>0</v>
       </c>
@@ -6864,6 +7137,9 @@
       <c r="B433" s="1">
         <v>73</v>
       </c>
+      <c r="C433">
+        <v>0</v>
+      </c>
       <c r="D433">
         <v>0</v>
       </c>
@@ -6878,6 +7154,9 @@
       <c r="B434" s="1">
         <v>74</v>
       </c>
+      <c r="C434">
+        <v>0</v>
+      </c>
       <c r="D434">
         <v>0</v>
       </c>
@@ -6892,6 +7171,9 @@
       <c r="B435" s="1">
         <v>74</v>
       </c>
+      <c r="C435">
+        <v>0</v>
+      </c>
       <c r="D435">
         <v>0</v>
       </c>
@@ -6906,6 +7188,9 @@
       <c r="B436" s="1">
         <v>74</v>
       </c>
+      <c r="C436">
+        <v>0</v>
+      </c>
       <c r="D436">
         <v>0</v>
       </c>
@@ -6920,6 +7205,9 @@
       <c r="B437" s="1">
         <v>74</v>
       </c>
+      <c r="C437">
+        <v>0</v>
+      </c>
       <c r="D437">
         <v>0</v>
       </c>
@@ -6934,6 +7222,9 @@
       <c r="B438" s="1">
         <v>75</v>
       </c>
+      <c r="C438">
+        <v>0</v>
+      </c>
       <c r="D438">
         <v>0</v>
       </c>
@@ -6948,6 +7239,9 @@
       <c r="B439" s="1">
         <v>75</v>
       </c>
+      <c r="C439">
+        <v>0</v>
+      </c>
       <c r="D439">
         <v>0</v>
       </c>
@@ -6962,6 +7256,9 @@
       <c r="B440" s="1">
         <v>75</v>
       </c>
+      <c r="C440">
+        <v>0</v>
+      </c>
       <c r="D440">
         <v>0</v>
       </c>
@@ -6976,6 +7273,9 @@
       <c r="B441" s="1">
         <v>75</v>
       </c>
+      <c r="C441">
+        <v>0</v>
+      </c>
       <c r="D441">
         <v>0</v>
       </c>
@@ -6990,6 +7290,9 @@
       <c r="B442" s="1">
         <v>76</v>
       </c>
+      <c r="C442">
+        <v>0</v>
+      </c>
       <c r="D442">
         <v>0</v>
       </c>
@@ -7004,6 +7307,9 @@
       <c r="B443" s="1">
         <v>76</v>
       </c>
+      <c r="C443">
+        <v>0</v>
+      </c>
       <c r="D443">
         <v>0</v>
       </c>
@@ -7018,6 +7324,9 @@
       <c r="B444" s="1">
         <v>76</v>
       </c>
+      <c r="C444">
+        <v>0</v>
+      </c>
       <c r="D444">
         <v>0</v>
       </c>
@@ -7032,6 +7341,9 @@
       <c r="B445" s="1">
         <v>76</v>
       </c>
+      <c r="C445">
+        <v>0</v>
+      </c>
       <c r="D445">
         <v>0</v>
       </c>
@@ -7046,6 +7358,9 @@
       <c r="B446" s="1">
         <v>77</v>
       </c>
+      <c r="C446">
+        <v>0</v>
+      </c>
       <c r="D446">
         <v>0</v>
       </c>
@@ -7060,6 +7375,9 @@
       <c r="B447" s="1">
         <v>77</v>
       </c>
+      <c r="C447">
+        <v>0</v>
+      </c>
       <c r="D447">
         <v>0</v>
       </c>
@@ -7074,6 +7392,9 @@
       <c r="B448" s="1">
         <v>77</v>
       </c>
+      <c r="C448">
+        <v>0</v>
+      </c>
       <c r="D448">
         <v>0</v>
       </c>
@@ -7088,6 +7409,9 @@
       <c r="B449" s="1">
         <v>77</v>
       </c>
+      <c r="C449">
+        <v>0</v>
+      </c>
       <c r="D449">
         <v>0</v>
       </c>
@@ -7102,6 +7426,9 @@
       <c r="B450" s="1">
         <v>78</v>
       </c>
+      <c r="C450">
+        <v>0</v>
+      </c>
       <c r="D450">
         <v>0</v>
       </c>
@@ -7116,6 +7443,9 @@
       <c r="B451" s="1">
         <v>78</v>
       </c>
+      <c r="C451">
+        <v>0</v>
+      </c>
       <c r="D451">
         <v>0</v>
       </c>
@@ -7130,6 +7460,9 @@
       <c r="B452" s="1">
         <v>78</v>
       </c>
+      <c r="C452">
+        <v>0</v>
+      </c>
       <c r="D452">
         <v>0</v>
       </c>
@@ -7144,6 +7477,9 @@
       <c r="B453" s="1">
         <v>78</v>
       </c>
+      <c r="C453">
+        <v>0</v>
+      </c>
       <c r="D453">
         <v>0</v>
       </c>
@@ -7158,6 +7494,9 @@
       <c r="B454" s="1">
         <v>79</v>
       </c>
+      <c r="C454">
+        <v>0</v>
+      </c>
       <c r="D454">
         <v>0</v>
       </c>
@@ -7172,6 +7511,9 @@
       <c r="B455" s="1">
         <v>79</v>
       </c>
+      <c r="C455">
+        <v>0</v>
+      </c>
       <c r="D455">
         <v>0</v>
       </c>
@@ -7186,6 +7528,9 @@
       <c r="B456" s="1">
         <v>79</v>
       </c>
+      <c r="C456">
+        <v>0</v>
+      </c>
       <c r="D456">
         <v>0</v>
       </c>
@@ -7200,6 +7545,9 @@
       <c r="B457" s="1">
         <v>79</v>
       </c>
+      <c r="C457">
+        <v>0</v>
+      </c>
       <c r="D457">
         <v>0</v>
       </c>
@@ -7214,6 +7562,9 @@
       <c r="B458" s="1">
         <v>80</v>
       </c>
+      <c r="C458">
+        <v>0</v>
+      </c>
       <c r="D458">
         <v>0</v>
       </c>
@@ -7228,6 +7579,9 @@
       <c r="B459" s="1">
         <v>80</v>
       </c>
+      <c r="C459">
+        <v>0</v>
+      </c>
       <c r="D459">
         <v>0</v>
       </c>
@@ -7242,6 +7596,9 @@
       <c r="B460" s="1">
         <v>80</v>
       </c>
+      <c r="C460">
+        <v>0</v>
+      </c>
       <c r="D460">
         <v>0</v>
       </c>
@@ -7256,6 +7613,9 @@
       <c r="B461" s="1">
         <v>80</v>
       </c>
+      <c r="C461">
+        <v>0</v>
+      </c>
       <c r="D461">
         <v>0</v>
       </c>
@@ -7270,6 +7630,9 @@
       <c r="B462" s="1">
         <v>81</v>
       </c>
+      <c r="C462">
+        <v>0</v>
+      </c>
       <c r="D462">
         <v>0</v>
       </c>
@@ -7284,6 +7647,9 @@
       <c r="B463" s="1">
         <v>81</v>
       </c>
+      <c r="C463">
+        <v>0</v>
+      </c>
       <c r="D463">
         <v>0</v>
       </c>
@@ -7298,6 +7664,9 @@
       <c r="B464" s="1">
         <v>81</v>
       </c>
+      <c r="C464">
+        <v>0</v>
+      </c>
       <c r="D464">
         <v>0</v>
       </c>
@@ -7312,6 +7681,9 @@
       <c r="B465" s="1">
         <v>81</v>
       </c>
+      <c r="C465">
+        <v>0</v>
+      </c>
       <c r="D465">
         <v>0</v>
       </c>
@@ -7326,6 +7698,9 @@
       <c r="B466" s="1">
         <v>82</v>
       </c>
+      <c r="C466">
+        <v>0</v>
+      </c>
       <c r="D466">
         <v>0</v>
       </c>
@@ -7340,6 +7715,9 @@
       <c r="B467" s="1">
         <v>82</v>
       </c>
+      <c r="C467">
+        <v>0</v>
+      </c>
       <c r="D467">
         <v>0</v>
       </c>
@@ -7354,6 +7732,9 @@
       <c r="B468" s="1">
         <v>82</v>
       </c>
+      <c r="C468">
+        <v>0</v>
+      </c>
       <c r="D468">
         <v>0</v>
       </c>
@@ -7368,6 +7749,9 @@
       <c r="B469" s="1">
         <v>82</v>
       </c>
+      <c r="C469">
+        <v>0</v>
+      </c>
       <c r="D469">
         <v>0</v>
       </c>
@@ -7382,6 +7766,9 @@
       <c r="B470" s="1">
         <v>83</v>
       </c>
+      <c r="C470">
+        <v>0</v>
+      </c>
       <c r="D470">
         <v>0</v>
       </c>
@@ -7396,6 +7783,9 @@
       <c r="B471" s="1">
         <v>83</v>
       </c>
+      <c r="C471">
+        <v>0</v>
+      </c>
       <c r="D471">
         <v>0</v>
       </c>
@@ -7410,6 +7800,9 @@
       <c r="B472" s="1">
         <v>83</v>
       </c>
+      <c r="C472">
+        <v>0</v>
+      </c>
       <c r="D472">
         <v>0</v>
       </c>
@@ -7424,6 +7817,9 @@
       <c r="B473" s="1">
         <v>83</v>
       </c>
+      <c r="C473">
+        <v>0</v>
+      </c>
       <c r="D473">
         <v>0</v>
       </c>
@@ -7438,6 +7834,9 @@
       <c r="B474" s="1">
         <v>84</v>
       </c>
+      <c r="C474">
+        <v>0</v>
+      </c>
       <c r="D474">
         <v>0</v>
       </c>
@@ -7452,6 +7851,9 @@
       <c r="B475" s="1">
         <v>84</v>
       </c>
+      <c r="C475">
+        <v>0</v>
+      </c>
       <c r="D475">
         <v>0</v>
       </c>
@@ -7466,6 +7868,9 @@
       <c r="B476" s="1">
         <v>84</v>
       </c>
+      <c r="C476">
+        <v>0</v>
+      </c>
       <c r="D476">
         <v>0</v>
       </c>
@@ -7480,6 +7885,9 @@
       <c r="B477" s="1">
         <v>84</v>
       </c>
+      <c r="C477">
+        <v>0</v>
+      </c>
       <c r="D477">
         <v>0</v>
       </c>
@@ -7494,6 +7902,9 @@
       <c r="B478" s="1">
         <v>85</v>
       </c>
+      <c r="C478">
+        <v>0</v>
+      </c>
       <c r="D478">
         <v>0</v>
       </c>
@@ -7508,6 +7919,9 @@
       <c r="B479" s="1">
         <v>85</v>
       </c>
+      <c r="C479">
+        <v>0</v>
+      </c>
       <c r="D479">
         <v>0</v>
       </c>
@@ -7522,6 +7936,9 @@
       <c r="B480" s="1">
         <v>85</v>
       </c>
+      <c r="C480">
+        <v>0</v>
+      </c>
       <c r="D480">
         <v>0</v>
       </c>
@@ -7536,6 +7953,9 @@
       <c r="B481" s="1">
         <v>85</v>
       </c>
+      <c r="C481">
+        <v>0</v>
+      </c>
       <c r="D481">
         <v>0</v>
       </c>
@@ -7550,6 +7970,9 @@
       <c r="B482" s="1">
         <v>86</v>
       </c>
+      <c r="C482">
+        <v>0</v>
+      </c>
       <c r="D482">
         <v>0</v>
       </c>
@@ -7564,6 +7987,9 @@
       <c r="B483" s="1">
         <v>86</v>
       </c>
+      <c r="C483">
+        <v>0</v>
+      </c>
       <c r="D483">
         <v>0</v>
       </c>
@@ -7578,6 +8004,9 @@
       <c r="B484" s="1">
         <v>86</v>
       </c>
+      <c r="C484">
+        <v>0</v>
+      </c>
       <c r="D484">
         <v>0</v>
       </c>
@@ -7592,6 +8021,9 @@
       <c r="B485" s="1">
         <v>86</v>
       </c>
+      <c r="C485">
+        <v>0</v>
+      </c>
       <c r="D485">
         <v>0</v>
       </c>
@@ -7606,6 +8038,9 @@
       <c r="B486" s="1">
         <v>87</v>
       </c>
+      <c r="C486">
+        <v>0</v>
+      </c>
       <c r="D486">
         <v>0</v>
       </c>
@@ -7620,6 +8055,9 @@
       <c r="B487" s="1">
         <v>87</v>
       </c>
+      <c r="C487">
+        <v>0</v>
+      </c>
       <c r="D487">
         <v>0</v>
       </c>
@@ -7634,6 +8072,9 @@
       <c r="B488" s="1">
         <v>87</v>
       </c>
+      <c r="C488">
+        <v>0</v>
+      </c>
       <c r="D488">
         <v>0</v>
       </c>
@@ -7648,6 +8089,9 @@
       <c r="B489" s="1">
         <v>87</v>
       </c>
+      <c r="C489">
+        <v>0</v>
+      </c>
       <c r="D489">
         <v>0</v>
       </c>
@@ -7662,6 +8106,9 @@
       <c r="B490" s="1">
         <v>88</v>
       </c>
+      <c r="C490">
+        <v>0</v>
+      </c>
       <c r="D490">
         <v>0</v>
       </c>
@@ -7676,6 +8123,9 @@
       <c r="B491" s="1">
         <v>88</v>
       </c>
+      <c r="C491">
+        <v>0</v>
+      </c>
       <c r="D491">
         <v>0</v>
       </c>
@@ -7690,6 +8140,9 @@
       <c r="B492" s="1">
         <v>88</v>
       </c>
+      <c r="C492">
+        <v>0</v>
+      </c>
       <c r="D492">
         <v>0</v>
       </c>
@@ -7704,6 +8157,9 @@
       <c r="B493" s="1">
         <v>88</v>
       </c>
+      <c r="C493">
+        <v>0</v>
+      </c>
       <c r="D493">
         <v>0</v>
       </c>
@@ -7718,6 +8174,9 @@
       <c r="B494" s="1">
         <v>89</v>
       </c>
+      <c r="C494">
+        <v>0</v>
+      </c>
       <c r="D494">
         <v>0</v>
       </c>
@@ -7732,6 +8191,9 @@
       <c r="B495" s="1">
         <v>89</v>
       </c>
+      <c r="C495">
+        <v>0</v>
+      </c>
       <c r="D495">
         <v>0</v>
       </c>
@@ -7746,6 +8208,9 @@
       <c r="B496" s="1">
         <v>89</v>
       </c>
+      <c r="C496">
+        <v>0</v>
+      </c>
       <c r="D496">
         <v>0</v>
       </c>
@@ -7760,6 +8225,9 @@
       <c r="B497" s="1">
         <v>89</v>
       </c>
+      <c r="C497">
+        <v>0</v>
+      </c>
       <c r="D497">
         <v>0</v>
       </c>
@@ -7774,6 +8242,9 @@
       <c r="B498" s="1">
         <v>90</v>
       </c>
+      <c r="C498">
+        <v>0</v>
+      </c>
       <c r="D498">
         <v>0</v>
       </c>
@@ -7788,6 +8259,9 @@
       <c r="B499" s="1">
         <v>90</v>
       </c>
+      <c r="C499">
+        <v>0</v>
+      </c>
       <c r="D499">
         <v>0</v>
       </c>
@@ -7802,6 +8276,9 @@
       <c r="B500" s="1">
         <v>90</v>
       </c>
+      <c r="C500">
+        <v>0</v>
+      </c>
       <c r="D500">
         <v>0</v>
       </c>
@@ -7816,6 +8293,9 @@
       <c r="B501" s="1">
         <v>90</v>
       </c>
+      <c r="C501">
+        <v>0</v>
+      </c>
       <c r="D501">
         <v>0</v>
       </c>
@@ -7830,6 +8310,9 @@
       <c r="B502" s="1">
         <v>91</v>
       </c>
+      <c r="C502">
+        <v>0</v>
+      </c>
       <c r="D502">
         <v>0</v>
       </c>
@@ -7844,6 +8327,9 @@
       <c r="B503" s="1">
         <v>91</v>
       </c>
+      <c r="C503">
+        <v>0</v>
+      </c>
       <c r="D503">
         <v>0</v>
       </c>
@@ -7858,6 +8344,9 @@
       <c r="B504" s="1">
         <v>91</v>
       </c>
+      <c r="C504">
+        <v>0</v>
+      </c>
       <c r="D504">
         <v>0</v>
       </c>
@@ -7872,6 +8361,9 @@
       <c r="B505" s="1">
         <v>91</v>
       </c>
+      <c r="C505">
+        <v>0</v>
+      </c>
       <c r="D505">
         <v>0</v>
       </c>
@@ -7886,6 +8378,9 @@
       <c r="B506" s="1">
         <v>92</v>
       </c>
+      <c r="C506">
+        <v>0</v>
+      </c>
       <c r="D506">
         <v>0</v>
       </c>
@@ -7900,6 +8395,9 @@
       <c r="B507" s="1">
         <v>92</v>
       </c>
+      <c r="C507">
+        <v>0</v>
+      </c>
       <c r="D507">
         <v>0</v>
       </c>
@@ -7914,6 +8412,9 @@
       <c r="B508" s="1">
         <v>92</v>
       </c>
+      <c r="C508">
+        <v>0</v>
+      </c>
       <c r="D508">
         <v>0</v>
       </c>
@@ -7928,6 +8429,9 @@
       <c r="B509" s="1">
         <v>92</v>
       </c>
+      <c r="C509">
+        <v>0</v>
+      </c>
       <c r="D509">
         <v>0</v>
       </c>
@@ -7942,6 +8446,9 @@
       <c r="B510" s="1">
         <v>93</v>
       </c>
+      <c r="C510">
+        <v>0</v>
+      </c>
       <c r="D510">
         <v>0</v>
       </c>
@@ -7956,6 +8463,9 @@
       <c r="B511" s="1">
         <v>93</v>
       </c>
+      <c r="C511">
+        <v>0</v>
+      </c>
       <c r="D511">
         <v>0</v>
       </c>
@@ -7970,6 +8480,9 @@
       <c r="B512" s="1">
         <v>93</v>
       </c>
+      <c r="C512">
+        <v>0</v>
+      </c>
       <c r="D512">
         <v>0</v>
       </c>
@@ -7984,6 +8497,9 @@
       <c r="B513" s="1">
         <v>93</v>
       </c>
+      <c r="C513">
+        <v>0</v>
+      </c>
       <c r="D513">
         <v>0</v>
       </c>
@@ -7998,6 +8514,9 @@
       <c r="B514" s="1">
         <v>94</v>
       </c>
+      <c r="C514">
+        <v>0</v>
+      </c>
       <c r="D514">
         <v>0</v>
       </c>
@@ -8012,6 +8531,9 @@
       <c r="B515" s="1">
         <v>94</v>
       </c>
+      <c r="C515">
+        <v>0</v>
+      </c>
       <c r="D515">
         <v>0</v>
       </c>
@@ -8026,6 +8548,9 @@
       <c r="B516" s="1">
         <v>94</v>
       </c>
+      <c r="C516">
+        <v>0</v>
+      </c>
       <c r="D516">
         <v>0</v>
       </c>
@@ -8040,6 +8565,9 @@
       <c r="B517" s="1">
         <v>94</v>
       </c>
+      <c r="C517">
+        <v>0</v>
+      </c>
       <c r="D517">
         <v>0</v>
       </c>
@@ -8054,6 +8582,9 @@
       <c r="B518" s="1">
         <v>95</v>
       </c>
+      <c r="C518">
+        <v>0</v>
+      </c>
       <c r="D518">
         <v>0</v>
       </c>
@@ -8068,6 +8599,9 @@
       <c r="B519" s="1">
         <v>95</v>
       </c>
+      <c r="C519">
+        <v>0</v>
+      </c>
       <c r="D519">
         <v>0</v>
       </c>
@@ -8082,6 +8616,9 @@
       <c r="B520" s="1">
         <v>95</v>
       </c>
+      <c r="C520">
+        <v>0</v>
+      </c>
       <c r="D520">
         <v>0</v>
       </c>
@@ -8096,6 +8633,9 @@
       <c r="B521" s="1">
         <v>95</v>
       </c>
+      <c r="C521">
+        <v>0</v>
+      </c>
       <c r="D521">
         <v>0</v>
       </c>
@@ -8110,6 +8650,9 @@
       <c r="B522" s="1">
         <v>96</v>
       </c>
+      <c r="C522">
+        <v>0</v>
+      </c>
       <c r="D522">
         <v>0</v>
       </c>
@@ -8124,6 +8667,9 @@
       <c r="B523" s="1">
         <v>96</v>
       </c>
+      <c r="C523">
+        <v>0</v>
+      </c>
       <c r="D523">
         <v>0</v>
       </c>
@@ -8138,6 +8684,9 @@
       <c r="B524" s="1">
         <v>96</v>
       </c>
+      <c r="C524">
+        <v>0</v>
+      </c>
       <c r="D524">
         <v>0</v>
       </c>
@@ -8152,6 +8701,9 @@
       <c r="B525" s="1">
         <v>96</v>
       </c>
+      <c r="C525">
+        <v>0</v>
+      </c>
       <c r="D525">
         <v>0</v>
       </c>
@@ -8166,6 +8718,9 @@
       <c r="B526" s="1">
         <v>97</v>
       </c>
+      <c r="C526">
+        <v>0</v>
+      </c>
       <c r="D526">
         <v>0</v>
       </c>
@@ -8180,6 +8735,9 @@
       <c r="B527" s="1">
         <v>97</v>
       </c>
+      <c r="C527">
+        <v>0</v>
+      </c>
       <c r="D527">
         <v>0</v>
       </c>
@@ -8194,6 +8752,9 @@
       <c r="B528" s="1">
         <v>97</v>
       </c>
+      <c r="C528">
+        <v>0</v>
+      </c>
       <c r="D528">
         <v>0</v>
       </c>
@@ -8208,6 +8769,9 @@
       <c r="B529" s="1">
         <v>97</v>
       </c>
+      <c r="C529">
+        <v>0</v>
+      </c>
       <c r="D529">
         <v>0</v>
       </c>
@@ -8222,6 +8786,9 @@
       <c r="B530" s="1">
         <v>98</v>
       </c>
+      <c r="C530">
+        <v>0</v>
+      </c>
       <c r="D530">
         <v>0</v>
       </c>
@@ -8236,6 +8803,9 @@
       <c r="B531" s="1">
         <v>98</v>
       </c>
+      <c r="C531">
+        <v>0</v>
+      </c>
       <c r="D531">
         <v>0</v>
       </c>
@@ -8250,6 +8820,9 @@
       <c r="B532" s="1">
         <v>98</v>
       </c>
+      <c r="C532">
+        <v>0</v>
+      </c>
       <c r="D532">
         <v>0</v>
       </c>
@@ -8263,6 +8836,9 @@
       </c>
       <c r="B533" s="1">
         <v>98</v>
+      </c>
+      <c r="C533">
+        <v>0</v>
       </c>
       <c r="D533">
         <v>0</v>

</xml_diff>

<commit_message>
now calls ending balance manual
</commit_message>
<xml_diff>
--- a/tranchedata.xlsx
+++ b/tranchedata.xlsx
@@ -495,10 +495,10 @@
         <v>1973564.140573333</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>94485124.06601793</v>
       </c>
       <c r="E5">
-        <v>361495416</v>
+        <v>267010291.9339821</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -507,13 +507,13 @@
         <v>51</v>
       </c>
       <c r="C6">
-        <v>1909900.7812</v>
+        <v>1410704.375717872</v>
       </c>
       <c r="D6">
-        <v>14916211.36000001</v>
+        <v>0</v>
       </c>
       <c r="E6">
-        <v>346579204.64</v>
+        <v>267010291.9339821</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -522,13 +522,13 @@
         <v>52</v>
       </c>
       <c r="C7">
-        <v>1892129.913331822</v>
+        <v>1457727.854908468</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7">
-        <v>346579204.64</v>
+        <v>267010291.9339821</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -537,13 +537,13 @@
         <v>53</v>
       </c>
       <c r="C8">
-        <v>1892129.913331822</v>
+        <v>1457727.854908468</v>
       </c>
       <c r="D8">
-        <v>65221702.36000001</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>281357502.28</v>
+        <v>267010291.9339821</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -552,13 +552,13 @@
         <v>54</v>
       </c>
       <c r="C9">
-        <v>1387405.105687378</v>
+        <v>1316657.41733668</v>
       </c>
       <c r="D9">
-        <v>55000000</v>
+        <v>11650000</v>
       </c>
       <c r="E9">
-        <v>226357502.28</v>
+        <v>255360291.9339821</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -567,13 +567,13 @@
         <v>55</v>
       </c>
       <c r="C10">
-        <v>1235786.208280866</v>
+        <v>1394125.32713069</v>
       </c>
       <c r="D10">
-        <v>58111292.09213597</v>
+        <v>14916211.36000001</v>
       </c>
       <c r="E10">
-        <v>168246210.187864</v>
+        <v>240444080.5739821</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -582,13 +582,13 @@
         <v>56</v>
       </c>
       <c r="C11">
-        <v>888900.8104925482</v>
+        <v>1270346.225699205</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>64667166.12400001</v>
       </c>
       <c r="E11">
-        <v>168246210.187864</v>
+        <v>175776914.449982</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -597,13 +597,13 @@
         <v>57</v>
       </c>
       <c r="C12">
-        <v>918530.8375089663</v>
+        <v>959644.2990555409</v>
       </c>
       <c r="D12">
-        <v>143686931.94</v>
+        <v>0</v>
       </c>
       <c r="E12">
-        <v>24559278.24786399</v>
+        <v>175776914.449982</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -612,13 +612,13 @@
         <v>58</v>
       </c>
       <c r="C13">
-        <v>129754.8534095481</v>
+        <v>928688.0313440718</v>
       </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>24559278.24786399</v>
+        <v>175776914.449982</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -627,13 +627,13 @@
         <v>59</v>
       </c>
       <c r="C14">
-        <v>134080.0151898663</v>
+        <v>959644.2990555409</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>65221702.36</v>
       </c>
       <c r="E14">
-        <v>24559278.24786399</v>
+        <v>110555212.089982</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -642,13 +642,13 @@
         <v>60</v>
       </c>
       <c r="C15">
-        <v>134080.0151898663</v>
+        <v>603570.0384490298</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>52552749.77999999</v>
       </c>
       <c r="E15">
-        <v>24559278.24786399</v>
+        <v>58002462.30998205</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -657,13 +657,13 @@
         <v>61</v>
       </c>
       <c r="C16">
-        <v>129754.8534095481</v>
+        <v>306446.3425377385</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>55000000</v>
       </c>
       <c r="E16">
-        <v>24559278.24786399</v>
+        <v>3002462.309982054</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -672,13 +672,13 @@
         <v>62</v>
       </c>
       <c r="C17">
-        <v>134080.0151898663</v>
+        <v>16391.77617788536</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>3002462.309982054</v>
       </c>
       <c r="E17">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -687,13 +687,13 @@
         <v>63</v>
       </c>
       <c r="C18">
-        <v>129754.8534095481</v>
+        <v>0</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -702,13 +702,13 @@
         <v>64</v>
       </c>
       <c r="C19">
-        <v>134080.0151898663</v>
+        <v>0</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -717,13 +717,13 @@
         <v>65</v>
       </c>
       <c r="C20">
-        <v>134080.0151898663</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -732,13 +732,13 @@
         <v>66</v>
       </c>
       <c r="C21">
-        <v>121104.5298489115</v>
+        <v>0</v>
       </c>
       <c r="D21">
         <v>0</v>
       </c>
       <c r="E21">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -747,13 +747,13 @@
         <v>67</v>
       </c>
       <c r="C22">
-        <v>134080.0151898663</v>
+        <v>0</v>
       </c>
       <c r="D22">
         <v>0</v>
       </c>
       <c r="E22">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -762,13 +762,13 @@
         <v>68</v>
       </c>
       <c r="C23">
-        <v>129754.8534095481</v>
+        <v>0</v>
       </c>
       <c r="D23">
         <v>0</v>
       </c>
       <c r="E23">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -777,13 +777,13 @@
         <v>69</v>
       </c>
       <c r="C24">
-        <v>134080.0151898663</v>
+        <v>0</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -792,13 +792,13 @@
         <v>70</v>
       </c>
       <c r="C25">
-        <v>129754.8534095481</v>
+        <v>0</v>
       </c>
       <c r="D25">
         <v>0</v>
       </c>
       <c r="E25">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -807,13 +807,13 @@
         <v>71</v>
       </c>
       <c r="C26">
-        <v>134080.0151898663</v>
+        <v>0</v>
       </c>
       <c r="D26">
         <v>0</v>
       </c>
       <c r="E26">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -822,13 +822,13 @@
         <v>72</v>
       </c>
       <c r="C27">
-        <v>134080.0151898663</v>
+        <v>0</v>
       </c>
       <c r="D27">
         <v>0</v>
       </c>
       <c r="E27">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -837,13 +837,13 @@
         <v>73</v>
       </c>
       <c r="C28">
-        <v>129754.8534095481</v>
+        <v>0</v>
       </c>
       <c r="D28">
         <v>0</v>
       </c>
       <c r="E28">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -852,13 +852,13 @@
         <v>74</v>
       </c>
       <c r="C29">
-        <v>134080.0151898663</v>
+        <v>0</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -867,13 +867,13 @@
         <v>75</v>
       </c>
       <c r="C30">
-        <v>129754.8534095481</v>
+        <v>0</v>
       </c>
       <c r="D30">
         <v>0</v>
       </c>
       <c r="E30">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -882,13 +882,13 @@
         <v>76</v>
       </c>
       <c r="C31">
-        <v>134080.0151898663</v>
+        <v>0</v>
       </c>
       <c r="D31">
         <v>0</v>
       </c>
       <c r="E31">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -897,13 +897,13 @@
         <v>77</v>
       </c>
       <c r="C32">
-        <v>134080.0151898663</v>
+        <v>0</v>
       </c>
       <c r="D32">
         <v>0</v>
       </c>
       <c r="E32">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -912,13 +912,13 @@
         <v>78</v>
       </c>
       <c r="C33">
-        <v>121104.5298489115</v>
+        <v>0</v>
       </c>
       <c r="D33">
         <v>0</v>
       </c>
       <c r="E33">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -927,13 +927,13 @@
         <v>79</v>
       </c>
       <c r="C34">
-        <v>134080.0151898663</v>
+        <v>0</v>
       </c>
       <c r="D34">
         <v>0</v>
       </c>
       <c r="E34">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -942,13 +942,13 @@
         <v>80</v>
       </c>
       <c r="C35">
-        <v>129754.8534095481</v>
+        <v>0</v>
       </c>
       <c r="D35">
         <v>0</v>
       </c>
       <c r="E35">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -957,13 +957,13 @@
         <v>81</v>
       </c>
       <c r="C36">
-        <v>134080.0151898663</v>
+        <v>0</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="E36">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -972,13 +972,13 @@
         <v>82</v>
       </c>
       <c r="C37">
-        <v>129754.8534095481</v>
+        <v>0</v>
       </c>
       <c r="D37">
         <v>0</v>
       </c>
       <c r="E37">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -987,13 +987,13 @@
         <v>83</v>
       </c>
       <c r="C38">
-        <v>134080.0151898663</v>
+        <v>0</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
       <c r="E38">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1002,13 +1002,13 @@
         <v>84</v>
       </c>
       <c r="C39">
-        <v>134080.0151898663</v>
+        <v>0</v>
       </c>
       <c r="D39">
         <v>0</v>
       </c>
       <c r="E39">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1017,13 +1017,13 @@
         <v>85</v>
       </c>
       <c r="C40">
-        <v>129754.8534095481</v>
+        <v>0</v>
       </c>
       <c r="D40">
         <v>0</v>
       </c>
       <c r="E40">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1032,13 +1032,13 @@
         <v>86</v>
       </c>
       <c r="C41">
-        <v>134080.0151898663</v>
+        <v>0</v>
       </c>
       <c r="D41">
         <v>0</v>
       </c>
       <c r="E41">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1047,13 +1047,13 @@
         <v>87</v>
       </c>
       <c r="C42">
-        <v>129754.8534095481</v>
+        <v>0</v>
       </c>
       <c r="D42">
         <v>0</v>
       </c>
       <c r="E42">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1062,13 +1062,13 @@
         <v>88</v>
       </c>
       <c r="C43">
-        <v>134080.0151898663</v>
+        <v>0</v>
       </c>
       <c r="D43">
         <v>0</v>
       </c>
       <c r="E43">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1077,13 +1077,13 @@
         <v>89</v>
       </c>
       <c r="C44">
-        <v>134080.0151898663</v>
+        <v>0</v>
       </c>
       <c r="D44">
         <v>0</v>
       </c>
       <c r="E44">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1092,13 +1092,13 @@
         <v>90</v>
       </c>
       <c r="C45">
-        <v>121104.5298489115</v>
+        <v>0</v>
       </c>
       <c r="D45">
         <v>0</v>
       </c>
       <c r="E45">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1107,13 +1107,13 @@
         <v>91</v>
       </c>
       <c r="C46">
-        <v>134080.0151898663</v>
+        <v>0</v>
       </c>
       <c r="D46">
         <v>0</v>
       </c>
       <c r="E46">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1122,13 +1122,13 @@
         <v>92</v>
       </c>
       <c r="C47">
-        <v>129754.8534095481</v>
+        <v>0</v>
       </c>
       <c r="D47">
         <v>0</v>
       </c>
       <c r="E47">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1137,13 +1137,13 @@
         <v>93</v>
       </c>
       <c r="C48">
-        <v>134080.0151898663</v>
+        <v>0</v>
       </c>
       <c r="D48">
         <v>0</v>
       </c>
       <c r="E48">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1152,13 +1152,13 @@
         <v>94</v>
       </c>
       <c r="C49">
-        <v>129754.8534095481</v>
+        <v>0</v>
       </c>
       <c r="D49">
         <v>0</v>
       </c>
       <c r="E49">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1167,13 +1167,13 @@
         <v>95</v>
       </c>
       <c r="C50">
-        <v>134080.0151898663</v>
+        <v>0</v>
       </c>
       <c r="D50">
         <v>0</v>
       </c>
       <c r="E50">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1182,13 +1182,13 @@
         <v>96</v>
       </c>
       <c r="C51">
-        <v>134080.0151898663</v>
+        <v>0</v>
       </c>
       <c r="D51">
         <v>0</v>
       </c>
       <c r="E51">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1197,13 +1197,13 @@
         <v>97</v>
       </c>
       <c r="C52">
-        <v>129754.8534095481</v>
+        <v>0</v>
       </c>
       <c r="D52">
         <v>0</v>
       </c>
       <c r="E52">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1212,13 +1212,13 @@
         <v>98</v>
       </c>
       <c r="C53">
-        <v>134080.0151898663</v>
+        <v>0</v>
       </c>
       <c r="D53">
         <v>0</v>
       </c>
       <c r="E53">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1227,13 +1227,13 @@
         <v>99</v>
       </c>
       <c r="C54">
-        <v>129754.8534095481</v>
+        <v>0</v>
       </c>
       <c r="D54">
         <v>0</v>
       </c>
       <c r="E54">
-        <v>24559278.24786399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1472,10 +1472,10 @@
         <v>812219.3749999999</v>
       </c>
       <c r="D70">
-        <v>0</v>
+        <v>87497537.69001794</v>
       </c>
       <c r="E70">
-        <v>141625000</v>
+        <v>54127462.30998206</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -1484,13 +1484,13 @@
         <v>63</v>
       </c>
       <c r="C71">
-        <v>786018.7499999999</v>
+        <v>300407.4158204004</v>
       </c>
       <c r="D71">
-        <v>0</v>
+        <v>54127462.30998206</v>
       </c>
       <c r="E71">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -1499,13 +1499,13 @@
         <v>64</v>
       </c>
       <c r="C72">
-        <v>812219.3749999999</v>
+        <v>0</v>
       </c>
       <c r="D72">
         <v>0</v>
       </c>
       <c r="E72">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -1514,13 +1514,13 @@
         <v>65</v>
       </c>
       <c r="C73">
-        <v>812219.3749999999</v>
+        <v>0</v>
       </c>
       <c r="D73">
         <v>0</v>
       </c>
       <c r="E73">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -1529,13 +1529,13 @@
         <v>66</v>
       </c>
       <c r="C74">
-        <v>733617.4999999999</v>
+        <v>0</v>
       </c>
       <c r="D74">
         <v>0</v>
       </c>
       <c r="E74">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -1544,13 +1544,13 @@
         <v>67</v>
       </c>
       <c r="C75">
-        <v>812219.3749999999</v>
+        <v>0</v>
       </c>
       <c r="D75">
         <v>0</v>
       </c>
       <c r="E75">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -1559,13 +1559,13 @@
         <v>68</v>
       </c>
       <c r="C76">
-        <v>786018.7499999999</v>
+        <v>0</v>
       </c>
       <c r="D76">
         <v>0</v>
       </c>
       <c r="E76">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -1574,13 +1574,13 @@
         <v>69</v>
       </c>
       <c r="C77">
-        <v>812219.3749999999</v>
+        <v>0</v>
       </c>
       <c r="D77">
         <v>0</v>
       </c>
       <c r="E77">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -1589,13 +1589,13 @@
         <v>70</v>
       </c>
       <c r="C78">
-        <v>786018.7499999999</v>
+        <v>0</v>
       </c>
       <c r="D78">
         <v>0</v>
       </c>
       <c r="E78">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -1604,13 +1604,13 @@
         <v>71</v>
       </c>
       <c r="C79">
-        <v>812219.3749999999</v>
+        <v>0</v>
       </c>
       <c r="D79">
         <v>0</v>
       </c>
       <c r="E79">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -1619,13 +1619,13 @@
         <v>72</v>
       </c>
       <c r="C80">
-        <v>812219.3749999999</v>
+        <v>0</v>
       </c>
       <c r="D80">
         <v>0</v>
       </c>
       <c r="E80">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -1634,13 +1634,13 @@
         <v>73</v>
       </c>
       <c r="C81">
-        <v>786018.7499999999</v>
+        <v>0</v>
       </c>
       <c r="D81">
         <v>0</v>
       </c>
       <c r="E81">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -1649,13 +1649,13 @@
         <v>74</v>
       </c>
       <c r="C82">
-        <v>812219.3749999999</v>
+        <v>0</v>
       </c>
       <c r="D82">
         <v>0</v>
       </c>
       <c r="E82">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -1664,13 +1664,13 @@
         <v>75</v>
       </c>
       <c r="C83">
-        <v>786018.7499999999</v>
+        <v>0</v>
       </c>
       <c r="D83">
         <v>0</v>
       </c>
       <c r="E83">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -1679,13 +1679,13 @@
         <v>76</v>
       </c>
       <c r="C84">
-        <v>812219.3749999999</v>
+        <v>0</v>
       </c>
       <c r="D84">
         <v>0</v>
       </c>
       <c r="E84">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -1694,13 +1694,13 @@
         <v>77</v>
       </c>
       <c r="C85">
-        <v>812219.3749999999</v>
+        <v>0</v>
       </c>
       <c r="D85">
         <v>0</v>
       </c>
       <c r="E85">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -1709,13 +1709,13 @@
         <v>78</v>
       </c>
       <c r="C86">
-        <v>733617.4999999999</v>
+        <v>0</v>
       </c>
       <c r="D86">
         <v>0</v>
       </c>
       <c r="E86">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -1724,13 +1724,13 @@
         <v>79</v>
       </c>
       <c r="C87">
-        <v>812219.3749999999</v>
+        <v>0</v>
       </c>
       <c r="D87">
         <v>0</v>
       </c>
       <c r="E87">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -1739,13 +1739,13 @@
         <v>80</v>
       </c>
       <c r="C88">
-        <v>786018.7499999999</v>
+        <v>0</v>
       </c>
       <c r="D88">
         <v>0</v>
       </c>
       <c r="E88">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -1754,13 +1754,13 @@
         <v>81</v>
       </c>
       <c r="C89">
-        <v>812219.3749999999</v>
+        <v>0</v>
       </c>
       <c r="D89">
         <v>0</v>
       </c>
       <c r="E89">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -1769,13 +1769,13 @@
         <v>82</v>
       </c>
       <c r="C90">
-        <v>786018.7499999999</v>
+        <v>0</v>
       </c>
       <c r="D90">
         <v>0</v>
       </c>
       <c r="E90">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -1784,13 +1784,13 @@
         <v>83</v>
       </c>
       <c r="C91">
-        <v>812219.3749999999</v>
+        <v>0</v>
       </c>
       <c r="D91">
         <v>0</v>
       </c>
       <c r="E91">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -1799,13 +1799,13 @@
         <v>84</v>
       </c>
       <c r="C92">
-        <v>812219.3749999999</v>
+        <v>0</v>
       </c>
       <c r="D92">
         <v>0</v>
       </c>
       <c r="E92">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -1814,13 +1814,13 @@
         <v>85</v>
       </c>
       <c r="C93">
-        <v>786018.7499999999</v>
+        <v>0</v>
       </c>
       <c r="D93">
         <v>0</v>
       </c>
       <c r="E93">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -1829,13 +1829,13 @@
         <v>86</v>
       </c>
       <c r="C94">
-        <v>812219.3749999999</v>
+        <v>0</v>
       </c>
       <c r="D94">
         <v>0</v>
       </c>
       <c r="E94">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -1844,13 +1844,13 @@
         <v>87</v>
       </c>
       <c r="C95">
-        <v>786018.7499999999</v>
+        <v>0</v>
       </c>
       <c r="D95">
         <v>0</v>
       </c>
       <c r="E95">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -1859,13 +1859,13 @@
         <v>88</v>
       </c>
       <c r="C96">
-        <v>812219.3749999999</v>
+        <v>0</v>
       </c>
       <c r="D96">
         <v>0</v>
       </c>
       <c r="E96">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -1874,13 +1874,13 @@
         <v>89</v>
       </c>
       <c r="C97">
-        <v>812219.3749999999</v>
+        <v>0</v>
       </c>
       <c r="D97">
         <v>0</v>
       </c>
       <c r="E97">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -1889,13 +1889,13 @@
         <v>90</v>
       </c>
       <c r="C98">
-        <v>733617.4999999999</v>
+        <v>0</v>
       </c>
       <c r="D98">
         <v>0</v>
       </c>
       <c r="E98">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -1904,13 +1904,13 @@
         <v>91</v>
       </c>
       <c r="C99">
-        <v>812219.3749999999</v>
+        <v>0</v>
       </c>
       <c r="D99">
         <v>0</v>
       </c>
       <c r="E99">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -1919,13 +1919,13 @@
         <v>92</v>
       </c>
       <c r="C100">
-        <v>786018.7499999999</v>
+        <v>0</v>
       </c>
       <c r="D100">
         <v>0</v>
       </c>
       <c r="E100">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -1934,13 +1934,13 @@
         <v>93</v>
       </c>
       <c r="C101">
-        <v>812219.3749999999</v>
+        <v>0</v>
       </c>
       <c r="D101">
         <v>0</v>
       </c>
       <c r="E101">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -1949,13 +1949,13 @@
         <v>94</v>
       </c>
       <c r="C102">
-        <v>786018.7499999999</v>
+        <v>0</v>
       </c>
       <c r="D102">
         <v>0</v>
       </c>
       <c r="E102">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -1964,13 +1964,13 @@
         <v>95</v>
       </c>
       <c r="C103">
-        <v>812219.3749999999</v>
+        <v>0</v>
       </c>
       <c r="D103">
         <v>0</v>
       </c>
       <c r="E103">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -1979,13 +1979,13 @@
         <v>96</v>
       </c>
       <c r="C104">
-        <v>812219.3749999999</v>
+        <v>0</v>
       </c>
       <c r="D104">
         <v>0</v>
       </c>
       <c r="E104">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -1994,13 +1994,13 @@
         <v>97</v>
       </c>
       <c r="C105">
-        <v>786018.7499999999</v>
+        <v>0</v>
       </c>
       <c r="D105">
         <v>0</v>
       </c>
       <c r="E105">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2009,13 +2009,13 @@
         <v>98</v>
       </c>
       <c r="C106">
-        <v>812219.3749999999</v>
+        <v>0</v>
       </c>
       <c r="D106">
         <v>0</v>
       </c>
       <c r="E106">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2024,13 +2024,13 @@
         <v>99</v>
       </c>
       <c r="C107">
-        <v>786018.7499999999</v>
+        <v>0</v>
       </c>
       <c r="D107">
         <v>0</v>
       </c>
       <c r="E107">
-        <v>141625000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -2284,10 +2284,10 @@
         <v>377300</v>
       </c>
       <c r="D124">
-        <v>0</v>
+        <v>3983829.78215389</v>
       </c>
       <c r="E124">
-        <v>66000000</v>
+        <v>62016170.21784611</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -2296,13 +2296,13 @@
         <v>64</v>
       </c>
       <c r="C125">
-        <v>389876.6666666667</v>
+        <v>366343.2988479764</v>
       </c>
       <c r="D125">
-        <v>0</v>
+        <v>10204238.35</v>
       </c>
       <c r="E125">
-        <v>66000000</v>
+        <v>51811931.86784611</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -2311,13 +2311,13 @@
         <v>65</v>
       </c>
       <c r="C126">
-        <v>389876.6666666667</v>
+        <v>306064.5953060043</v>
       </c>
       <c r="D126">
         <v>0</v>
       </c>
       <c r="E126">
-        <v>66000000</v>
+        <v>51811931.86784611</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -2326,13 +2326,13 @@
         <v>66</v>
       </c>
       <c r="C127">
-        <v>352146.6666666667</v>
+        <v>276445.4409215522</v>
       </c>
       <c r="D127">
         <v>0</v>
       </c>
       <c r="E127">
-        <v>66000000</v>
+        <v>51811931.86784611</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -2341,13 +2341,13 @@
         <v>67</v>
       </c>
       <c r="C128">
-        <v>389876.6666666667</v>
+        <v>306064.5953060043</v>
       </c>
       <c r="D128">
-        <v>0</v>
+        <v>51811931.86784611</v>
       </c>
       <c r="E128">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -2356,13 +2356,13 @@
         <v>68</v>
       </c>
       <c r="C129">
-        <v>377300</v>
+        <v>0</v>
       </c>
       <c r="D129">
         <v>0</v>
       </c>
       <c r="E129">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -2371,13 +2371,13 @@
         <v>69</v>
       </c>
       <c r="C130">
-        <v>389876.6666666667</v>
+        <v>0</v>
       </c>
       <c r="D130">
         <v>0</v>
       </c>
       <c r="E130">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -2386,13 +2386,13 @@
         <v>70</v>
       </c>
       <c r="C131">
-        <v>377300</v>
+        <v>0</v>
       </c>
       <c r="D131">
         <v>0</v>
       </c>
       <c r="E131">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -2401,13 +2401,13 @@
         <v>71</v>
       </c>
       <c r="C132">
-        <v>389876.6666666667</v>
+        <v>0</v>
       </c>
       <c r="D132">
         <v>0</v>
       </c>
       <c r="E132">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -2416,13 +2416,13 @@
         <v>72</v>
       </c>
       <c r="C133">
-        <v>389876.6666666667</v>
+        <v>0</v>
       </c>
       <c r="D133">
         <v>0</v>
       </c>
       <c r="E133">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -2431,13 +2431,13 @@
         <v>73</v>
       </c>
       <c r="C134">
-        <v>377300</v>
+        <v>0</v>
       </c>
       <c r="D134">
         <v>0</v>
       </c>
       <c r="E134">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -2446,13 +2446,13 @@
         <v>74</v>
       </c>
       <c r="C135">
-        <v>389876.6666666667</v>
+        <v>0</v>
       </c>
       <c r="D135">
         <v>0</v>
       </c>
       <c r="E135">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -2461,13 +2461,13 @@
         <v>75</v>
       </c>
       <c r="C136">
-        <v>377300</v>
+        <v>0</v>
       </c>
       <c r="D136">
         <v>0</v>
       </c>
       <c r="E136">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -2476,13 +2476,13 @@
         <v>76</v>
       </c>
       <c r="C137">
-        <v>389876.6666666667</v>
+        <v>0</v>
       </c>
       <c r="D137">
         <v>0</v>
       </c>
       <c r="E137">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -2491,13 +2491,13 @@
         <v>77</v>
       </c>
       <c r="C138">
-        <v>389876.6666666667</v>
+        <v>0</v>
       </c>
       <c r="D138">
         <v>0</v>
       </c>
       <c r="E138">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -2506,13 +2506,13 @@
         <v>78</v>
       </c>
       <c r="C139">
-        <v>352146.6666666667</v>
+        <v>0</v>
       </c>
       <c r="D139">
         <v>0</v>
       </c>
       <c r="E139">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -2521,13 +2521,13 @@
         <v>79</v>
       </c>
       <c r="C140">
-        <v>389876.6666666667</v>
+        <v>0</v>
       </c>
       <c r="D140">
         <v>0</v>
       </c>
       <c r="E140">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -2536,13 +2536,13 @@
         <v>80</v>
       </c>
       <c r="C141">
-        <v>377300</v>
+        <v>0</v>
       </c>
       <c r="D141">
         <v>0</v>
       </c>
       <c r="E141">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -2551,13 +2551,13 @@
         <v>81</v>
       </c>
       <c r="C142">
-        <v>389876.6666666667</v>
+        <v>0</v>
       </c>
       <c r="D142">
         <v>0</v>
       </c>
       <c r="E142">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -2566,13 +2566,13 @@
         <v>82</v>
       </c>
       <c r="C143">
-        <v>377300</v>
+        <v>0</v>
       </c>
       <c r="D143">
         <v>0</v>
       </c>
       <c r="E143">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -2581,13 +2581,13 @@
         <v>83</v>
       </c>
       <c r="C144">
-        <v>389876.6666666667</v>
+        <v>0</v>
       </c>
       <c r="D144">
         <v>0</v>
       </c>
       <c r="E144">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -2596,13 +2596,13 @@
         <v>84</v>
       </c>
       <c r="C145">
-        <v>389876.6666666667</v>
+        <v>0</v>
       </c>
       <c r="D145">
         <v>0</v>
       </c>
       <c r="E145">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -2611,13 +2611,13 @@
         <v>85</v>
       </c>
       <c r="C146">
-        <v>377300</v>
+        <v>0</v>
       </c>
       <c r="D146">
         <v>0</v>
       </c>
       <c r="E146">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -2626,13 +2626,13 @@
         <v>86</v>
       </c>
       <c r="C147">
-        <v>389876.6666666667</v>
+        <v>0</v>
       </c>
       <c r="D147">
         <v>0</v>
       </c>
       <c r="E147">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -2641,13 +2641,13 @@
         <v>87</v>
       </c>
       <c r="C148">
-        <v>377300</v>
+        <v>0</v>
       </c>
       <c r="D148">
         <v>0</v>
       </c>
       <c r="E148">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -2656,13 +2656,13 @@
         <v>88</v>
       </c>
       <c r="C149">
-        <v>389876.6666666667</v>
+        <v>0</v>
       </c>
       <c r="D149">
         <v>0</v>
       </c>
       <c r="E149">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -2671,13 +2671,13 @@
         <v>89</v>
       </c>
       <c r="C150">
-        <v>389876.6666666667</v>
+        <v>0</v>
       </c>
       <c r="D150">
         <v>0</v>
       </c>
       <c r="E150">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -2686,13 +2686,13 @@
         <v>90</v>
       </c>
       <c r="C151">
-        <v>352146.6666666667</v>
+        <v>0</v>
       </c>
       <c r="D151">
         <v>0</v>
       </c>
       <c r="E151">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -2701,13 +2701,13 @@
         <v>91</v>
       </c>
       <c r="C152">
-        <v>389876.6666666667</v>
+        <v>0</v>
       </c>
       <c r="D152">
         <v>0</v>
       </c>
       <c r="E152">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -2716,13 +2716,13 @@
         <v>92</v>
       </c>
       <c r="C153">
-        <v>377300</v>
+        <v>0</v>
       </c>
       <c r="D153">
         <v>0</v>
       </c>
       <c r="E153">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -2731,13 +2731,13 @@
         <v>93</v>
       </c>
       <c r="C154">
-        <v>389876.6666666667</v>
+        <v>0</v>
       </c>
       <c r="D154">
         <v>0</v>
       </c>
       <c r="E154">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="155" spans="1:5">
@@ -2746,13 +2746,13 @@
         <v>94</v>
       </c>
       <c r="C155">
-        <v>377300</v>
+        <v>0</v>
       </c>
       <c r="D155">
         <v>0</v>
       </c>
       <c r="E155">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -2761,13 +2761,13 @@
         <v>95</v>
       </c>
       <c r="C156">
-        <v>389876.6666666667</v>
+        <v>0</v>
       </c>
       <c r="D156">
         <v>0</v>
       </c>
       <c r="E156">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157" spans="1:5">
@@ -2776,13 +2776,13 @@
         <v>96</v>
       </c>
       <c r="C157">
-        <v>389876.6666666667</v>
+        <v>0</v>
       </c>
       <c r="D157">
         <v>0</v>
       </c>
       <c r="E157">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158" spans="1:5">
@@ -2791,13 +2791,13 @@
         <v>97</v>
       </c>
       <c r="C158">
-        <v>377300</v>
+        <v>0</v>
       </c>
       <c r="D158">
         <v>0</v>
       </c>
       <c r="E158">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159" spans="1:5">
@@ -2806,13 +2806,13 @@
         <v>98</v>
       </c>
       <c r="C159">
-        <v>389876.6666666667</v>
+        <v>0</v>
       </c>
       <c r="D159">
         <v>0</v>
       </c>
       <c r="E159">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160" spans="1:5">
@@ -2821,13 +2821,13 @@
         <v>99</v>
       </c>
       <c r="C160">
-        <v>377300</v>
+        <v>0</v>
       </c>
       <c r="D160">
         <v>0</v>
       </c>
       <c r="E160">
-        <v>66000000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161" spans="1:5">
@@ -3141,10 +3141,10 @@
         <v>495136.7361111111</v>
       </c>
       <c r="D181">
-        <v>0</v>
+        <v>79750000</v>
       </c>
       <c r="E181">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="182" spans="1:5">
@@ -3153,13 +3153,13 @@
         <v>68</v>
       </c>
       <c r="C182">
-        <v>479164.5833333333</v>
+        <v>0</v>
       </c>
       <c r="D182">
         <v>0</v>
       </c>
       <c r="E182">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="183" spans="1:5">
@@ -3168,13 +3168,13 @@
         <v>69</v>
       </c>
       <c r="C183">
-        <v>495136.7361111111</v>
+        <v>0</v>
       </c>
       <c r="D183">
         <v>0</v>
       </c>
       <c r="E183">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="184" spans="1:5">
@@ -3183,13 +3183,13 @@
         <v>70</v>
       </c>
       <c r="C184">
-        <v>479164.5833333333</v>
+        <v>0</v>
       </c>
       <c r="D184">
         <v>0</v>
       </c>
       <c r="E184">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="185" spans="1:5">
@@ -3198,13 +3198,13 @@
         <v>71</v>
       </c>
       <c r="C185">
-        <v>495136.7361111111</v>
+        <v>0</v>
       </c>
       <c r="D185">
         <v>0</v>
       </c>
       <c r="E185">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="186" spans="1:5">
@@ -3213,13 +3213,13 @@
         <v>72</v>
       </c>
       <c r="C186">
-        <v>495136.7361111111</v>
+        <v>0</v>
       </c>
       <c r="D186">
         <v>0</v>
       </c>
       <c r="E186">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="187" spans="1:5">
@@ -3228,13 +3228,13 @@
         <v>73</v>
       </c>
       <c r="C187">
-        <v>479164.5833333333</v>
+        <v>0</v>
       </c>
       <c r="D187">
         <v>0</v>
       </c>
       <c r="E187">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="188" spans="1:5">
@@ -3243,13 +3243,13 @@
         <v>74</v>
       </c>
       <c r="C188">
-        <v>495136.7361111111</v>
+        <v>0</v>
       </c>
       <c r="D188">
         <v>0</v>
       </c>
       <c r="E188">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189" spans="1:5">
@@ -3258,13 +3258,13 @@
         <v>75</v>
       </c>
       <c r="C189">
-        <v>479164.5833333333</v>
+        <v>0</v>
       </c>
       <c r="D189">
         <v>0</v>
       </c>
       <c r="E189">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="190" spans="1:5">
@@ -3273,13 +3273,13 @@
         <v>76</v>
       </c>
       <c r="C190">
-        <v>495136.7361111111</v>
+        <v>0</v>
       </c>
       <c r="D190">
         <v>0</v>
       </c>
       <c r="E190">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="191" spans="1:5">
@@ -3288,13 +3288,13 @@
         <v>77</v>
       </c>
       <c r="C191">
-        <v>495136.7361111111</v>
+        <v>0</v>
       </c>
       <c r="D191">
         <v>0</v>
       </c>
       <c r="E191">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="192" spans="1:5">
@@ -3303,13 +3303,13 @@
         <v>78</v>
       </c>
       <c r="C192">
-        <v>447220.2777777778</v>
+        <v>0</v>
       </c>
       <c r="D192">
         <v>0</v>
       </c>
       <c r="E192">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193" spans="1:5">
@@ -3318,13 +3318,13 @@
         <v>79</v>
       </c>
       <c r="C193">
-        <v>495136.7361111111</v>
+        <v>0</v>
       </c>
       <c r="D193">
         <v>0</v>
       </c>
       <c r="E193">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="194" spans="1:5">
@@ -3333,13 +3333,13 @@
         <v>80</v>
       </c>
       <c r="C194">
-        <v>479164.5833333333</v>
+        <v>0</v>
       </c>
       <c r="D194">
         <v>0</v>
       </c>
       <c r="E194">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="195" spans="1:5">
@@ -3348,13 +3348,13 @@
         <v>81</v>
       </c>
       <c r="C195">
-        <v>495136.7361111111</v>
+        <v>0</v>
       </c>
       <c r="D195">
         <v>0</v>
       </c>
       <c r="E195">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="196" spans="1:5">
@@ -3363,13 +3363,13 @@
         <v>82</v>
       </c>
       <c r="C196">
-        <v>479164.5833333333</v>
+        <v>0</v>
       </c>
       <c r="D196">
         <v>0</v>
       </c>
       <c r="E196">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -3378,13 +3378,13 @@
         <v>83</v>
       </c>
       <c r="C197">
-        <v>495136.7361111111</v>
+        <v>0</v>
       </c>
       <c r="D197">
         <v>0</v>
       </c>
       <c r="E197">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="198" spans="1:5">
@@ -3393,13 +3393,13 @@
         <v>84</v>
       </c>
       <c r="C198">
-        <v>495136.7361111111</v>
+        <v>0</v>
       </c>
       <c r="D198">
         <v>0</v>
       </c>
       <c r="E198">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="199" spans="1:5">
@@ -3408,13 +3408,13 @@
         <v>85</v>
       </c>
       <c r="C199">
-        <v>479164.5833333333</v>
+        <v>0</v>
       </c>
       <c r="D199">
         <v>0</v>
       </c>
       <c r="E199">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="200" spans="1:5">
@@ -3423,13 +3423,13 @@
         <v>86</v>
       </c>
       <c r="C200">
-        <v>495136.7361111111</v>
+        <v>0</v>
       </c>
       <c r="D200">
         <v>0</v>
       </c>
       <c r="E200">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="201" spans="1:5">
@@ -3438,13 +3438,13 @@
         <v>87</v>
       </c>
       <c r="C201">
-        <v>479164.5833333333</v>
+        <v>0</v>
       </c>
       <c r="D201">
         <v>0</v>
       </c>
       <c r="E201">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="202" spans="1:5">
@@ -3453,13 +3453,13 @@
         <v>88</v>
       </c>
       <c r="C202">
-        <v>495136.7361111111</v>
+        <v>0</v>
       </c>
       <c r="D202">
         <v>0</v>
       </c>
       <c r="E202">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="203" spans="1:5">
@@ -3468,13 +3468,13 @@
         <v>89</v>
       </c>
       <c r="C203">
-        <v>495136.7361111111</v>
+        <v>0</v>
       </c>
       <c r="D203">
         <v>0</v>
       </c>
       <c r="E203">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="204" spans="1:5">
@@ -3483,13 +3483,13 @@
         <v>90</v>
       </c>
       <c r="C204">
-        <v>447220.2777777778</v>
+        <v>0</v>
       </c>
       <c r="D204">
         <v>0</v>
       </c>
       <c r="E204">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="205" spans="1:5">
@@ -3498,13 +3498,13 @@
         <v>91</v>
       </c>
       <c r="C205">
-        <v>495136.7361111111</v>
+        <v>0</v>
       </c>
       <c r="D205">
         <v>0</v>
       </c>
       <c r="E205">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -3513,13 +3513,13 @@
         <v>92</v>
       </c>
       <c r="C206">
-        <v>479164.5833333333</v>
+        <v>0</v>
       </c>
       <c r="D206">
         <v>0</v>
       </c>
       <c r="E206">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="207" spans="1:5">
@@ -3528,13 +3528,13 @@
         <v>93</v>
       </c>
       <c r="C207">
-        <v>495136.7361111111</v>
+        <v>0</v>
       </c>
       <c r="D207">
         <v>0</v>
       </c>
       <c r="E207">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="208" spans="1:5">
@@ -3543,13 +3543,13 @@
         <v>94</v>
       </c>
       <c r="C208">
-        <v>479164.5833333333</v>
+        <v>0</v>
       </c>
       <c r="D208">
         <v>0</v>
       </c>
       <c r="E208">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="209" spans="1:5">
@@ -3558,13 +3558,13 @@
         <v>95</v>
       </c>
       <c r="C209">
-        <v>495136.7361111111</v>
+        <v>0</v>
       </c>
       <c r="D209">
         <v>0</v>
       </c>
       <c r="E209">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -3573,13 +3573,13 @@
         <v>96</v>
       </c>
       <c r="C210">
-        <v>495136.7361111111</v>
+        <v>0</v>
       </c>
       <c r="D210">
         <v>0</v>
       </c>
       <c r="E210">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="211" spans="1:5">
@@ -3588,13 +3588,13 @@
         <v>97</v>
       </c>
       <c r="C211">
-        <v>479164.5833333333</v>
+        <v>0</v>
       </c>
       <c r="D211">
         <v>0</v>
       </c>
       <c r="E211">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="212" spans="1:5">
@@ -3603,13 +3603,13 @@
         <v>98</v>
       </c>
       <c r="C212">
-        <v>495136.7361111111</v>
+        <v>0</v>
       </c>
       <c r="D212">
         <v>0</v>
       </c>
       <c r="E212">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="213" spans="1:5">
@@ -3618,13 +3618,13 @@
         <v>99</v>
       </c>
       <c r="C213">
-        <v>479164.5833333333</v>
+        <v>0</v>
       </c>
       <c r="D213">
         <v>0</v>
       </c>
       <c r="E213">
-        <v>79750000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="214" spans="1:5">
@@ -3938,10 +3938,10 @@
         <v>387449.4097222222</v>
       </c>
       <c r="D234">
-        <v>0</v>
+        <v>12125000.07215391</v>
       </c>
       <c r="E234">
-        <v>59125000</v>
+        <v>46999999.92784609</v>
       </c>
     </row>
     <row r="235" spans="1:5">
@@ -3950,13 +3950,13 @@
         <v>68</v>
       </c>
       <c r="C235">
-        <v>374951.0416666667</v>
+        <v>298058.3328757573</v>
       </c>
       <c r="D235">
         <v>0</v>
       </c>
       <c r="E235">
-        <v>59125000</v>
+        <v>46999999.92784609</v>
       </c>
     </row>
     <row r="236" spans="1:5">
@@ -3965,13 +3965,13 @@
         <v>69</v>
       </c>
       <c r="C236">
-        <v>387449.4097222222</v>
+        <v>307993.6106382826</v>
       </c>
       <c r="D236">
         <v>0</v>
       </c>
       <c r="E236">
-        <v>59125000</v>
+        <v>46999999.92784609</v>
       </c>
     </row>
     <row r="237" spans="1:5">
@@ -3980,13 +3980,13 @@
         <v>70</v>
       </c>
       <c r="C237">
-        <v>374951.0416666667</v>
+        <v>298058.3328757573</v>
       </c>
       <c r="D237">
         <v>0</v>
       </c>
       <c r="E237">
-        <v>59125000</v>
+        <v>46999999.92784609</v>
       </c>
     </row>
     <row r="238" spans="1:5">
@@ -3995,13 +3995,13 @@
         <v>71</v>
       </c>
       <c r="C238">
-        <v>387449.4097222222</v>
+        <v>307993.6106382826</v>
       </c>
       <c r="D238">
         <v>0</v>
       </c>
       <c r="E238">
-        <v>59125000</v>
+        <v>46999999.92784609</v>
       </c>
     </row>
     <row r="239" spans="1:5">
@@ -4010,13 +4010,13 @@
         <v>72</v>
       </c>
       <c r="C239">
-        <v>387449.4097222222</v>
+        <v>307993.6106382826</v>
       </c>
       <c r="D239">
         <v>0</v>
       </c>
       <c r="E239">
-        <v>59125000</v>
+        <v>46999999.92784609</v>
       </c>
     </row>
     <row r="240" spans="1:5">
@@ -4025,13 +4025,13 @@
         <v>73</v>
       </c>
       <c r="C240">
-        <v>374951.0416666667</v>
+        <v>298058.3328757573</v>
       </c>
       <c r="D240">
         <v>0</v>
       </c>
       <c r="E240">
-        <v>59125000</v>
+        <v>46999999.92784609</v>
       </c>
     </row>
     <row r="241" spans="1:5">
@@ -4040,13 +4040,13 @@
         <v>74</v>
       </c>
       <c r="C241">
-        <v>387449.4097222222</v>
+        <v>307993.6106382826</v>
       </c>
       <c r="D241">
         <v>0</v>
       </c>
       <c r="E241">
-        <v>59125000</v>
+        <v>46999999.92784609</v>
       </c>
     </row>
     <row r="242" spans="1:5">
@@ -4055,13 +4055,13 @@
         <v>75</v>
       </c>
       <c r="C242">
-        <v>374951.0416666667</v>
+        <v>298058.3328757573</v>
       </c>
       <c r="D242">
         <v>0</v>
       </c>
       <c r="E242">
-        <v>59125000</v>
+        <v>46999999.92784609</v>
       </c>
     </row>
     <row r="243" spans="1:5">
@@ -4070,13 +4070,13 @@
         <v>76</v>
       </c>
       <c r="C243">
-        <v>387449.4097222222</v>
+        <v>307993.6106382826</v>
       </c>
       <c r="D243">
         <v>0</v>
       </c>
       <c r="E243">
-        <v>59125000</v>
+        <v>46999999.92784609</v>
       </c>
     </row>
     <row r="244" spans="1:5">
@@ -4085,13 +4085,13 @@
         <v>77</v>
       </c>
       <c r="C244">
-        <v>387449.4097222222</v>
+        <v>307993.6106382826</v>
       </c>
       <c r="D244">
         <v>0</v>
       </c>
       <c r="E244">
-        <v>59125000</v>
+        <v>46999999.92784609</v>
       </c>
     </row>
     <row r="245" spans="1:5">
@@ -4100,13 +4100,13 @@
         <v>78</v>
       </c>
       <c r="C245">
-        <v>349954.3055555556</v>
+        <v>278187.7773507068</v>
       </c>
       <c r="D245">
         <v>0</v>
       </c>
       <c r="E245">
-        <v>59125000</v>
+        <v>46999999.92784609</v>
       </c>
     </row>
     <row r="246" spans="1:5">
@@ -4115,13 +4115,13 @@
         <v>79</v>
       </c>
       <c r="C246">
-        <v>387449.4097222222</v>
+        <v>307993.6106382826</v>
       </c>
       <c r="D246">
         <v>0</v>
       </c>
       <c r="E246">
-        <v>59125000</v>
+        <v>46999999.92784609</v>
       </c>
     </row>
     <row r="247" spans="1:5">
@@ -4130,13 +4130,13 @@
         <v>80</v>
       </c>
       <c r="C247">
-        <v>374951.0416666667</v>
+        <v>298058.3328757573</v>
       </c>
       <c r="D247">
-        <v>0</v>
+        <v>46999999.92784609</v>
       </c>
       <c r="E247">
-        <v>59125000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="248" spans="1:5">
@@ -4145,13 +4145,13 @@
         <v>81</v>
       </c>
       <c r="C248">
-        <v>387449.4097222222</v>
+        <v>0</v>
       </c>
       <c r="D248">
         <v>0</v>
       </c>
       <c r="E248">
-        <v>59125000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="249" spans="1:5">
@@ -4160,13 +4160,13 @@
         <v>82</v>
       </c>
       <c r="C249">
-        <v>374951.0416666667</v>
+        <v>0</v>
       </c>
       <c r="D249">
         <v>0</v>
       </c>
       <c r="E249">
-        <v>59125000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="250" spans="1:5">
@@ -4175,13 +4175,13 @@
         <v>83</v>
       </c>
       <c r="C250">
-        <v>387449.4097222222</v>
+        <v>0</v>
       </c>
       <c r="D250">
         <v>0</v>
       </c>
       <c r="E250">
-        <v>59125000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="251" spans="1:5">
@@ -4190,13 +4190,13 @@
         <v>84</v>
       </c>
       <c r="C251">
-        <v>387449.4097222222</v>
+        <v>0</v>
       </c>
       <c r="D251">
         <v>0</v>
       </c>
       <c r="E251">
-        <v>59125000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="252" spans="1:5">
@@ -4205,13 +4205,13 @@
         <v>85</v>
       </c>
       <c r="C252">
-        <v>374951.0416666667</v>
+        <v>0</v>
       </c>
       <c r="D252">
         <v>0</v>
       </c>
       <c r="E252">
-        <v>59125000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="253" spans="1:5">
@@ -4220,13 +4220,13 @@
         <v>86</v>
       </c>
       <c r="C253">
-        <v>387449.4097222222</v>
+        <v>0</v>
       </c>
       <c r="D253">
         <v>0</v>
       </c>
       <c r="E253">
-        <v>59125000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="254" spans="1:5">
@@ -4235,13 +4235,13 @@
         <v>87</v>
       </c>
       <c r="C254">
-        <v>374951.0416666667</v>
+        <v>0</v>
       </c>
       <c r="D254">
         <v>0</v>
       </c>
       <c r="E254">
-        <v>59125000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="255" spans="1:5">
@@ -4250,13 +4250,13 @@
         <v>88</v>
       </c>
       <c r="C255">
-        <v>387449.4097222222</v>
+        <v>0</v>
       </c>
       <c r="D255">
         <v>0</v>
       </c>
       <c r="E255">
-        <v>59125000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="256" spans="1:5">
@@ -4265,13 +4265,13 @@
         <v>89</v>
       </c>
       <c r="C256">
-        <v>387449.4097222222</v>
+        <v>0</v>
       </c>
       <c r="D256">
         <v>0</v>
       </c>
       <c r="E256">
-        <v>59125000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="257" spans="1:5">
@@ -4280,13 +4280,13 @@
         <v>90</v>
       </c>
       <c r="C257">
-        <v>349954.3055555556</v>
+        <v>0</v>
       </c>
       <c r="D257">
         <v>0</v>
       </c>
       <c r="E257">
-        <v>59125000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="258" spans="1:5">
@@ -4295,13 +4295,13 @@
         <v>91</v>
       </c>
       <c r="C258">
-        <v>387449.4097222222</v>
+        <v>0</v>
       </c>
       <c r="D258">
         <v>0</v>
       </c>
       <c r="E258">
-        <v>59125000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="259" spans="1:5">
@@ -4310,13 +4310,13 @@
         <v>92</v>
       </c>
       <c r="C259">
-        <v>374951.0416666667</v>
+        <v>0</v>
       </c>
       <c r="D259">
         <v>0</v>
       </c>
       <c r="E259">
-        <v>59125000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="260" spans="1:5">
@@ -4325,13 +4325,13 @@
         <v>93</v>
       </c>
       <c r="C260">
-        <v>387449.4097222222</v>
+        <v>0</v>
       </c>
       <c r="D260">
         <v>0</v>
       </c>
       <c r="E260">
-        <v>59125000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="261" spans="1:5">
@@ -4340,13 +4340,13 @@
         <v>94</v>
       </c>
       <c r="C261">
-        <v>374951.0416666667</v>
+        <v>0</v>
       </c>
       <c r="D261">
         <v>0</v>
       </c>
       <c r="E261">
-        <v>59125000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="262" spans="1:5">
@@ -4355,13 +4355,13 @@
         <v>95</v>
       </c>
       <c r="C262">
-        <v>387449.4097222222</v>
+        <v>0</v>
       </c>
       <c r="D262">
         <v>0</v>
       </c>
       <c r="E262">
-        <v>59125000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="263" spans="1:5">
@@ -4370,13 +4370,13 @@
         <v>96</v>
       </c>
       <c r="C263">
-        <v>387449.4097222222</v>
+        <v>0</v>
       </c>
       <c r="D263">
         <v>0</v>
       </c>
       <c r="E263">
-        <v>59125000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="264" spans="1:5">
@@ -4385,13 +4385,13 @@
         <v>97</v>
       </c>
       <c r="C264">
-        <v>374951.0416666667</v>
+        <v>0</v>
       </c>
       <c r="D264">
         <v>0</v>
       </c>
       <c r="E264">
-        <v>59125000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="265" spans="1:5">
@@ -4400,13 +4400,13 @@
         <v>98</v>
       </c>
       <c r="C265">
-        <v>387449.4097222222</v>
+        <v>0</v>
       </c>
       <c r="D265">
         <v>0</v>
       </c>
       <c r="E265">
-        <v>59125000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="266" spans="1:5">
@@ -4415,13 +4415,13 @@
         <v>99</v>
       </c>
       <c r="C266">
-        <v>374951.0416666667</v>
+        <v>0</v>
       </c>
       <c r="D266">
         <v>0</v>
       </c>
       <c r="E266">
-        <v>59125000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="267" spans="1:5">
@@ -4930,10 +4930,10 @@
         <v>82087.5</v>
       </c>
       <c r="D300">
-        <v>0</v>
+        <v>12375000</v>
       </c>
       <c r="E300">
-        <v>12375000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="301" spans="1:5">
@@ -4942,13 +4942,13 @@
         <v>81</v>
       </c>
       <c r="C301">
-        <v>84823.75</v>
+        <v>0</v>
       </c>
       <c r="D301">
         <v>0</v>
       </c>
       <c r="E301">
-        <v>12375000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="302" spans="1:5">
@@ -4957,13 +4957,13 @@
         <v>82</v>
       </c>
       <c r="C302">
-        <v>82087.5</v>
+        <v>0</v>
       </c>
       <c r="D302">
         <v>0</v>
       </c>
       <c r="E302">
-        <v>12375000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="303" spans="1:5">
@@ -4972,13 +4972,13 @@
         <v>83</v>
       </c>
       <c r="C303">
-        <v>84823.75</v>
+        <v>0</v>
       </c>
       <c r="D303">
         <v>0</v>
       </c>
       <c r="E303">
-        <v>12375000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="304" spans="1:5">
@@ -4987,13 +4987,13 @@
         <v>84</v>
       </c>
       <c r="C304">
-        <v>84823.75</v>
+        <v>0</v>
       </c>
       <c r="D304">
         <v>0</v>
       </c>
       <c r="E304">
-        <v>12375000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="305" spans="1:5">
@@ -5002,13 +5002,13 @@
         <v>85</v>
       </c>
       <c r="C305">
-        <v>82087.5</v>
+        <v>0</v>
       </c>
       <c r="D305">
         <v>0</v>
       </c>
       <c r="E305">
-        <v>12375000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="306" spans="1:5">
@@ -5017,13 +5017,13 @@
         <v>86</v>
       </c>
       <c r="C306">
-        <v>84823.75</v>
+        <v>0</v>
       </c>
       <c r="D306">
         <v>0</v>
       </c>
       <c r="E306">
-        <v>12375000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="307" spans="1:5">
@@ -5032,13 +5032,13 @@
         <v>87</v>
       </c>
       <c r="C307">
-        <v>82087.5</v>
+        <v>0</v>
       </c>
       <c r="D307">
         <v>0</v>
       </c>
       <c r="E307">
-        <v>12375000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="308" spans="1:5">
@@ -5047,13 +5047,13 @@
         <v>88</v>
       </c>
       <c r="C308">
-        <v>84823.75</v>
+        <v>0</v>
       </c>
       <c r="D308">
         <v>0</v>
       </c>
       <c r="E308">
-        <v>12375000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="309" spans="1:5">
@@ -5062,13 +5062,13 @@
         <v>89</v>
       </c>
       <c r="C309">
-        <v>84823.75</v>
+        <v>0</v>
       </c>
       <c r="D309">
         <v>0</v>
       </c>
       <c r="E309">
-        <v>12375000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="310" spans="1:5">
@@ -5077,13 +5077,13 @@
         <v>90</v>
       </c>
       <c r="C310">
-        <v>76615</v>
+        <v>0</v>
       </c>
       <c r="D310">
         <v>0</v>
       </c>
       <c r="E310">
-        <v>12375000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="311" spans="1:5">
@@ -5092,13 +5092,13 @@
         <v>91</v>
       </c>
       <c r="C311">
-        <v>84823.75</v>
+        <v>0</v>
       </c>
       <c r="D311">
         <v>0</v>
       </c>
       <c r="E311">
-        <v>12375000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="312" spans="1:5">
@@ -5107,13 +5107,13 @@
         <v>92</v>
       </c>
       <c r="C312">
-        <v>82087.5</v>
+        <v>0</v>
       </c>
       <c r="D312">
         <v>0</v>
       </c>
       <c r="E312">
-        <v>12375000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="313" spans="1:5">
@@ -5122,13 +5122,13 @@
         <v>93</v>
       </c>
       <c r="C313">
-        <v>84823.75</v>
+        <v>0</v>
       </c>
       <c r="D313">
         <v>0</v>
       </c>
       <c r="E313">
-        <v>12375000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="314" spans="1:5">
@@ -5137,13 +5137,13 @@
         <v>94</v>
       </c>
       <c r="C314">
-        <v>82087.5</v>
+        <v>0</v>
       </c>
       <c r="D314">
         <v>0</v>
       </c>
       <c r="E314">
-        <v>12375000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="315" spans="1:5">
@@ -5152,13 +5152,13 @@
         <v>95</v>
       </c>
       <c r="C315">
-        <v>84823.75</v>
+        <v>0</v>
       </c>
       <c r="D315">
         <v>0</v>
       </c>
       <c r="E315">
-        <v>12375000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="316" spans="1:5">
@@ -5167,13 +5167,13 @@
         <v>96</v>
       </c>
       <c r="C316">
-        <v>84823.75</v>
+        <v>0</v>
       </c>
       <c r="D316">
         <v>0</v>
       </c>
       <c r="E316">
-        <v>12375000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="317" spans="1:5">
@@ -5182,13 +5182,13 @@
         <v>97</v>
       </c>
       <c r="C317">
-        <v>82087.5</v>
+        <v>0</v>
       </c>
       <c r="D317">
         <v>0</v>
       </c>
       <c r="E317">
-        <v>12375000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="318" spans="1:5">
@@ -5197,13 +5197,13 @@
         <v>98</v>
       </c>
       <c r="C318">
-        <v>84823.75</v>
+        <v>0</v>
       </c>
       <c r="D318">
         <v>0</v>
       </c>
       <c r="E318">
-        <v>12375000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="319" spans="1:5">
@@ -5212,13 +5212,13 @@
         <v>99</v>
       </c>
       <c r="C319">
-        <v>82087.5</v>
+        <v>0</v>
       </c>
       <c r="D319">
         <v>0</v>
       </c>
       <c r="E319">
-        <v>12375000</v>
+        <v>0</v>
       </c>
     </row>
     <row r="320" spans="1:5">
@@ -7472,14 +7472,11 @@
       <c r="B452" s="1">
         <v>80</v>
       </c>
-      <c r="C452">
-        <v>0</v>
-      </c>
       <c r="D452">
-        <v>0</v>
+        <v>21625000.07215391</v>
       </c>
       <c r="E452">
-        <v>53625000</v>
+        <v>31999999.92784609</v>
       </c>
     </row>
     <row r="453" spans="1:5">
@@ -7489,9 +7486,6 @@
       <c r="B453" s="1">
         <v>80</v>
       </c>
-      <c r="C453">
-        <v>0</v>
-      </c>
       <c r="D453">
         <v>0</v>
       </c>
@@ -7506,9 +7500,6 @@
       <c r="B454" s="1">
         <v>80</v>
       </c>
-      <c r="C454">
-        <v>0</v>
-      </c>
       <c r="D454">
         <v>0</v>
       </c>
@@ -7523,9 +7514,6 @@
       <c r="B455" s="1">
         <v>80</v>
       </c>
-      <c r="C455">
-        <v>0</v>
-      </c>
       <c r="D455">
         <v>0</v>
       </c>
@@ -7540,14 +7528,11 @@
       <c r="B456" s="1">
         <v>81</v>
       </c>
-      <c r="C456">
-        <v>0</v>
-      </c>
       <c r="D456">
         <v>0</v>
       </c>
       <c r="E456">
-        <v>53625000</v>
+        <v>31999999.92784609</v>
       </c>
     </row>
     <row r="457" spans="1:5">
@@ -7557,9 +7542,6 @@
       <c r="B457" s="1">
         <v>81</v>
       </c>
-      <c r="C457">
-        <v>0</v>
-      </c>
       <c r="D457">
         <v>0</v>
       </c>
@@ -7574,9 +7556,6 @@
       <c r="B458" s="1">
         <v>81</v>
       </c>
-      <c r="C458">
-        <v>0</v>
-      </c>
       <c r="D458">
         <v>0</v>
       </c>
@@ -7591,9 +7570,6 @@
       <c r="B459" s="1">
         <v>81</v>
       </c>
-      <c r="C459">
-        <v>0</v>
-      </c>
       <c r="D459">
         <v>0</v>
       </c>
@@ -7608,14 +7584,11 @@
       <c r="B460" s="1">
         <v>82</v>
       </c>
-      <c r="C460">
-        <v>0</v>
-      </c>
       <c r="D460">
         <v>0</v>
       </c>
       <c r="E460">
-        <v>53625000</v>
+        <v>31999999.92784609</v>
       </c>
     </row>
     <row r="461" spans="1:5">
@@ -7625,9 +7598,6 @@
       <c r="B461" s="1">
         <v>82</v>
       </c>
-      <c r="C461">
-        <v>0</v>
-      </c>
       <c r="D461">
         <v>0</v>
       </c>
@@ -7642,9 +7612,6 @@
       <c r="B462" s="1">
         <v>82</v>
       </c>
-      <c r="C462">
-        <v>0</v>
-      </c>
       <c r="D462">
         <v>0</v>
       </c>
@@ -7659,9 +7626,6 @@
       <c r="B463" s="1">
         <v>82</v>
       </c>
-      <c r="C463">
-        <v>0</v>
-      </c>
       <c r="D463">
         <v>0</v>
       </c>
@@ -7676,14 +7640,11 @@
       <c r="B464" s="1">
         <v>83</v>
       </c>
-      <c r="C464">
-        <v>0</v>
-      </c>
       <c r="D464">
         <v>0</v>
       </c>
       <c r="E464">
-        <v>53625000</v>
+        <v>31999999.92784609</v>
       </c>
     </row>
     <row r="465" spans="1:5">
@@ -7693,9 +7654,6 @@
       <c r="B465" s="1">
         <v>83</v>
       </c>
-      <c r="C465">
-        <v>0</v>
-      </c>
       <c r="D465">
         <v>0</v>
       </c>
@@ -7710,9 +7668,6 @@
       <c r="B466" s="1">
         <v>83</v>
       </c>
-      <c r="C466">
-        <v>0</v>
-      </c>
       <c r="D466">
         <v>0</v>
       </c>
@@ -7727,9 +7682,6 @@
       <c r="B467" s="1">
         <v>83</v>
       </c>
-      <c r="C467">
-        <v>0</v>
-      </c>
       <c r="D467">
         <v>0</v>
       </c>
@@ -7744,14 +7696,11 @@
       <c r="B468" s="1">
         <v>84</v>
       </c>
-      <c r="C468">
-        <v>0</v>
-      </c>
       <c r="D468">
         <v>0</v>
       </c>
       <c r="E468">
-        <v>53625000</v>
+        <v>31999999.92784609</v>
       </c>
     </row>
     <row r="469" spans="1:5">
@@ -7761,9 +7710,6 @@
       <c r="B469" s="1">
         <v>84</v>
       </c>
-      <c r="C469">
-        <v>0</v>
-      </c>
       <c r="D469">
         <v>0</v>
       </c>
@@ -7778,9 +7724,6 @@
       <c r="B470" s="1">
         <v>84</v>
       </c>
-      <c r="C470">
-        <v>0</v>
-      </c>
       <c r="D470">
         <v>0</v>
       </c>
@@ -7795,9 +7738,6 @@
       <c r="B471" s="1">
         <v>84</v>
       </c>
-      <c r="C471">
-        <v>0</v>
-      </c>
       <c r="D471">
         <v>0</v>
       </c>
@@ -7812,14 +7752,11 @@
       <c r="B472" s="1">
         <v>85</v>
       </c>
-      <c r="C472">
-        <v>0</v>
-      </c>
       <c r="D472">
         <v>0</v>
       </c>
       <c r="E472">
-        <v>53625000</v>
+        <v>31999999.92784609</v>
       </c>
     </row>
     <row r="473" spans="1:5">
@@ -7829,9 +7766,6 @@
       <c r="B473" s="1">
         <v>85</v>
       </c>
-      <c r="C473">
-        <v>0</v>
-      </c>
       <c r="D473">
         <v>0</v>
       </c>
@@ -7846,9 +7780,6 @@
       <c r="B474" s="1">
         <v>85</v>
       </c>
-      <c r="C474">
-        <v>0</v>
-      </c>
       <c r="D474">
         <v>0</v>
       </c>
@@ -7863,9 +7794,6 @@
       <c r="B475" s="1">
         <v>85</v>
       </c>
-      <c r="C475">
-        <v>0</v>
-      </c>
       <c r="D475">
         <v>0</v>
       </c>
@@ -7880,14 +7808,11 @@
       <c r="B476" s="1">
         <v>86</v>
       </c>
-      <c r="C476">
-        <v>0</v>
-      </c>
       <c r="D476">
         <v>0</v>
       </c>
       <c r="E476">
-        <v>53625000</v>
+        <v>31999999.92784609</v>
       </c>
     </row>
     <row r="477" spans="1:5">
@@ -7897,9 +7822,6 @@
       <c r="B477" s="1">
         <v>86</v>
       </c>
-      <c r="C477">
-        <v>0</v>
-      </c>
       <c r="D477">
         <v>0</v>
       </c>
@@ -7914,9 +7836,6 @@
       <c r="B478" s="1">
         <v>86</v>
       </c>
-      <c r="C478">
-        <v>0</v>
-      </c>
       <c r="D478">
         <v>0</v>
       </c>
@@ -7931,9 +7850,6 @@
       <c r="B479" s="1">
         <v>86</v>
       </c>
-      <c r="C479">
-        <v>0</v>
-      </c>
       <c r="D479">
         <v>0</v>
       </c>
@@ -7948,14 +7864,11 @@
       <c r="B480" s="1">
         <v>87</v>
       </c>
-      <c r="C480">
-        <v>0</v>
-      </c>
       <c r="D480">
         <v>0</v>
       </c>
       <c r="E480">
-        <v>53625000</v>
+        <v>31999999.92784609</v>
       </c>
     </row>
     <row r="481" spans="1:5">
@@ -7965,9 +7878,6 @@
       <c r="B481" s="1">
         <v>87</v>
       </c>
-      <c r="C481">
-        <v>0</v>
-      </c>
       <c r="D481">
         <v>0</v>
       </c>
@@ -7982,9 +7892,6 @@
       <c r="B482" s="1">
         <v>87</v>
       </c>
-      <c r="C482">
-        <v>0</v>
-      </c>
       <c r="D482">
         <v>0</v>
       </c>
@@ -7999,9 +7906,6 @@
       <c r="B483" s="1">
         <v>87</v>
       </c>
-      <c r="C483">
-        <v>0</v>
-      </c>
       <c r="D483">
         <v>0</v>
       </c>
@@ -8016,14 +7920,11 @@
       <c r="B484" s="1">
         <v>88</v>
       </c>
-      <c r="C484">
-        <v>0</v>
-      </c>
       <c r="D484">
         <v>0</v>
       </c>
       <c r="E484">
-        <v>53625000</v>
+        <v>31999999.92784609</v>
       </c>
     </row>
     <row r="485" spans="1:5">
@@ -8033,9 +7934,6 @@
       <c r="B485" s="1">
         <v>88</v>
       </c>
-      <c r="C485">
-        <v>0</v>
-      </c>
       <c r="D485">
         <v>0</v>
       </c>
@@ -8050,9 +7948,6 @@
       <c r="B486" s="1">
         <v>88</v>
       </c>
-      <c r="C486">
-        <v>0</v>
-      </c>
       <c r="D486">
         <v>0</v>
       </c>
@@ -8067,9 +7962,6 @@
       <c r="B487" s="1">
         <v>88</v>
       </c>
-      <c r="C487">
-        <v>0</v>
-      </c>
       <c r="D487">
         <v>0</v>
       </c>
@@ -8084,14 +7976,11 @@
       <c r="B488" s="1">
         <v>89</v>
       </c>
-      <c r="C488">
-        <v>0</v>
-      </c>
       <c r="D488">
         <v>0</v>
       </c>
       <c r="E488">
-        <v>53625000</v>
+        <v>31999999.92784609</v>
       </c>
     </row>
     <row r="489" spans="1:5">
@@ -8101,9 +7990,6 @@
       <c r="B489" s="1">
         <v>89</v>
       </c>
-      <c r="C489">
-        <v>0</v>
-      </c>
       <c r="D489">
         <v>0</v>
       </c>
@@ -8118,9 +8004,6 @@
       <c r="B490" s="1">
         <v>89</v>
       </c>
-      <c r="C490">
-        <v>0</v>
-      </c>
       <c r="D490">
         <v>0</v>
       </c>
@@ -8135,9 +8018,6 @@
       <c r="B491" s="1">
         <v>89</v>
       </c>
-      <c r="C491">
-        <v>0</v>
-      </c>
       <c r="D491">
         <v>0</v>
       </c>
@@ -8152,14 +8032,11 @@
       <c r="B492" s="1">
         <v>90</v>
       </c>
-      <c r="C492">
-        <v>0</v>
-      </c>
       <c r="D492">
         <v>0</v>
       </c>
       <c r="E492">
-        <v>53625000</v>
+        <v>31999999.92784609</v>
       </c>
     </row>
     <row r="493" spans="1:5">
@@ -8169,9 +8046,6 @@
       <c r="B493" s="1">
         <v>90</v>
       </c>
-      <c r="C493">
-        <v>0</v>
-      </c>
       <c r="D493">
         <v>0</v>
       </c>
@@ -8186,9 +8060,6 @@
       <c r="B494" s="1">
         <v>90</v>
       </c>
-      <c r="C494">
-        <v>0</v>
-      </c>
       <c r="D494">
         <v>0</v>
       </c>
@@ -8203,9 +8074,6 @@
       <c r="B495" s="1">
         <v>90</v>
       </c>
-      <c r="C495">
-        <v>0</v>
-      </c>
       <c r="D495">
         <v>0</v>
       </c>
@@ -8220,14 +8088,11 @@
       <c r="B496" s="1">
         <v>91</v>
       </c>
-      <c r="C496">
-        <v>0</v>
-      </c>
       <c r="D496">
         <v>0</v>
       </c>
       <c r="E496">
-        <v>53625000</v>
+        <v>31999999.92784609</v>
       </c>
     </row>
     <row r="497" spans="1:5">
@@ -8237,9 +8102,6 @@
       <c r="B497" s="1">
         <v>91</v>
       </c>
-      <c r="C497">
-        <v>0</v>
-      </c>
       <c r="D497">
         <v>0</v>
       </c>
@@ -8254,9 +8116,6 @@
       <c r="B498" s="1">
         <v>91</v>
       </c>
-      <c r="C498">
-        <v>0</v>
-      </c>
       <c r="D498">
         <v>0</v>
       </c>
@@ -8271,9 +8130,6 @@
       <c r="B499" s="1">
         <v>91</v>
       </c>
-      <c r="C499">
-        <v>0</v>
-      </c>
       <c r="D499">
         <v>0</v>
       </c>
@@ -8288,14 +8144,11 @@
       <c r="B500" s="1">
         <v>92</v>
       </c>
-      <c r="C500">
-        <v>0</v>
-      </c>
       <c r="D500">
         <v>0</v>
       </c>
       <c r="E500">
-        <v>53625000</v>
+        <v>31999999.92784609</v>
       </c>
     </row>
     <row r="501" spans="1:5">
@@ -8305,9 +8158,6 @@
       <c r="B501" s="1">
         <v>92</v>
       </c>
-      <c r="C501">
-        <v>0</v>
-      </c>
       <c r="D501">
         <v>0</v>
       </c>
@@ -8322,9 +8172,6 @@
       <c r="B502" s="1">
         <v>92</v>
       </c>
-      <c r="C502">
-        <v>0</v>
-      </c>
       <c r="D502">
         <v>0</v>
       </c>
@@ -8339,9 +8186,6 @@
       <c r="B503" s="1">
         <v>92</v>
       </c>
-      <c r="C503">
-        <v>0</v>
-      </c>
       <c r="D503">
         <v>0</v>
       </c>
@@ -8356,14 +8200,11 @@
       <c r="B504" s="1">
         <v>93</v>
       </c>
-      <c r="C504">
-        <v>0</v>
-      </c>
       <c r="D504">
         <v>0</v>
       </c>
       <c r="E504">
-        <v>53625000</v>
+        <v>31999999.92784609</v>
       </c>
     </row>
     <row r="505" spans="1:5">
@@ -8373,9 +8214,6 @@
       <c r="B505" s="1">
         <v>93</v>
       </c>
-      <c r="C505">
-        <v>0</v>
-      </c>
       <c r="D505">
         <v>0</v>
       </c>
@@ -8390,9 +8228,6 @@
       <c r="B506" s="1">
         <v>93</v>
       </c>
-      <c r="C506">
-        <v>0</v>
-      </c>
       <c r="D506">
         <v>0</v>
       </c>
@@ -8407,9 +8242,6 @@
       <c r="B507" s="1">
         <v>93</v>
       </c>
-      <c r="C507">
-        <v>0</v>
-      </c>
       <c r="D507">
         <v>0</v>
       </c>
@@ -8424,14 +8256,11 @@
       <c r="B508" s="1">
         <v>94</v>
       </c>
-      <c r="C508">
-        <v>0</v>
-      </c>
       <c r="D508">
         <v>0</v>
       </c>
       <c r="E508">
-        <v>53625000</v>
+        <v>31999999.92784609</v>
       </c>
     </row>
     <row r="509" spans="1:5">
@@ -8441,9 +8270,6 @@
       <c r="B509" s="1">
         <v>94</v>
       </c>
-      <c r="C509">
-        <v>0</v>
-      </c>
       <c r="D509">
         <v>0</v>
       </c>
@@ -8458,9 +8284,6 @@
       <c r="B510" s="1">
         <v>94</v>
       </c>
-      <c r="C510">
-        <v>0</v>
-      </c>
       <c r="D510">
         <v>0</v>
       </c>
@@ -8475,9 +8298,6 @@
       <c r="B511" s="1">
         <v>94</v>
       </c>
-      <c r="C511">
-        <v>0</v>
-      </c>
       <c r="D511">
         <v>0</v>
       </c>
@@ -8492,14 +8312,11 @@
       <c r="B512" s="1">
         <v>95</v>
       </c>
-      <c r="C512">
-        <v>0</v>
-      </c>
       <c r="D512">
         <v>0</v>
       </c>
       <c r="E512">
-        <v>53625000</v>
+        <v>31999999.92784609</v>
       </c>
     </row>
     <row r="513" spans="1:5">
@@ -8509,9 +8326,6 @@
       <c r="B513" s="1">
         <v>95</v>
       </c>
-      <c r="C513">
-        <v>0</v>
-      </c>
       <c r="D513">
         <v>0</v>
       </c>
@@ -8526,9 +8340,6 @@
       <c r="B514" s="1">
         <v>95</v>
       </c>
-      <c r="C514">
-        <v>0</v>
-      </c>
       <c r="D514">
         <v>0</v>
       </c>
@@ -8543,9 +8354,6 @@
       <c r="B515" s="1">
         <v>95</v>
       </c>
-      <c r="C515">
-        <v>0</v>
-      </c>
       <c r="D515">
         <v>0</v>
       </c>
@@ -8560,14 +8368,11 @@
       <c r="B516" s="1">
         <v>96</v>
       </c>
-      <c r="C516">
-        <v>0</v>
-      </c>
       <c r="D516">
         <v>0</v>
       </c>
       <c r="E516">
-        <v>53625000</v>
+        <v>31999999.92784609</v>
       </c>
     </row>
     <row r="517" spans="1:5">
@@ -8577,9 +8382,6 @@
       <c r="B517" s="1">
         <v>96</v>
       </c>
-      <c r="C517">
-        <v>0</v>
-      </c>
       <c r="D517">
         <v>0</v>
       </c>
@@ -8594,9 +8396,6 @@
       <c r="B518" s="1">
         <v>96</v>
       </c>
-      <c r="C518">
-        <v>0</v>
-      </c>
       <c r="D518">
         <v>0</v>
       </c>
@@ -8611,9 +8410,6 @@
       <c r="B519" s="1">
         <v>96</v>
       </c>
-      <c r="C519">
-        <v>0</v>
-      </c>
       <c r="D519">
         <v>0</v>
       </c>
@@ -8628,14 +8424,11 @@
       <c r="B520" s="1">
         <v>97</v>
       </c>
-      <c r="C520">
-        <v>0</v>
-      </c>
       <c r="D520">
         <v>0</v>
       </c>
       <c r="E520">
-        <v>53625000</v>
+        <v>31999999.92784609</v>
       </c>
     </row>
     <row r="521" spans="1:5">
@@ -8645,9 +8438,6 @@
       <c r="B521" s="1">
         <v>97</v>
       </c>
-      <c r="C521">
-        <v>0</v>
-      </c>
       <c r="D521">
         <v>0</v>
       </c>
@@ -8662,9 +8452,6 @@
       <c r="B522" s="1">
         <v>97</v>
       </c>
-      <c r="C522">
-        <v>0</v>
-      </c>
       <c r="D522">
         <v>0</v>
       </c>
@@ -8679,9 +8466,6 @@
       <c r="B523" s="1">
         <v>97</v>
       </c>
-      <c r="C523">
-        <v>0</v>
-      </c>
       <c r="D523">
         <v>0</v>
       </c>
@@ -8696,14 +8480,11 @@
       <c r="B524" s="1">
         <v>98</v>
       </c>
-      <c r="C524">
-        <v>0</v>
-      </c>
       <c r="D524">
         <v>0</v>
       </c>
       <c r="E524">
-        <v>53625000</v>
+        <v>31999999.92784609</v>
       </c>
     </row>
     <row r="525" spans="1:5">
@@ -8713,9 +8494,6 @@
       <c r="B525" s="1">
         <v>98</v>
       </c>
-      <c r="C525">
-        <v>0</v>
-      </c>
       <c r="D525">
         <v>0</v>
       </c>
@@ -8730,9 +8508,6 @@
       <c r="B526" s="1">
         <v>98</v>
       </c>
-      <c r="C526">
-        <v>0</v>
-      </c>
       <c r="D526">
         <v>0</v>
       </c>
@@ -8747,9 +8522,6 @@
       <c r="B527" s="1">
         <v>98</v>
       </c>
-      <c r="C527">
-        <v>0</v>
-      </c>
       <c r="D527">
         <v>0</v>
       </c>
@@ -8768,7 +8540,7 @@
         <v>0</v>
       </c>
       <c r="E528">
-        <v>53625000</v>
+        <v>31999999.92784609</v>
       </c>
     </row>
     <row r="529" spans="1:5">

</xml_diff>